<commit_message>
add remaining life as a column in the data change ECL to forecast until remaining life, rather than remaining term. This allows the user to specify if they want to use remaining term or behavioural life.
</commit_message>
<xml_diff>
--- a/data/account_level_data.xlsx
+++ b/data/account_level_data.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\geyerbisschoff\PythonProjects\Z-model\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A585EC7-1D16-43FC-A19E-3A65BA27D65F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBD741DD-B6A5-4991-9E02-4DA774BDBA10}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1275" yWindow="-120" windowWidth="27645" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DATA" sheetId="1" r:id="rId1"/>
     <sheet name="DICTIONARY" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DATA!$A$1:$T$121</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DATA!$A$1:$U$121</definedName>
   </definedNames>
   <calcPr calcId="191029" calcOnSave="0"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="52">
   <si>
     <t>outstanding_balance</t>
   </si>
@@ -192,6 +192,9 @@
   <si>
     <t>watchlist</t>
   </si>
+  <si>
+    <t>remaining_life</t>
+  </si>
 </sst>
 </file>
 
@@ -275,7 +278,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="10">
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
@@ -284,6 +287,9 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
@@ -317,15 +323,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:U121" totalsRowShown="0">
-  <autoFilter ref="A1:U121" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="21">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="reporting_date" dataDxfId="8"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:V121" totalsRowShown="0">
+  <autoFilter ref="A1:V121" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="22">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="reporting_date" dataDxfId="9"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="contract_id"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="segment_id"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="origination_date" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="origination_date" dataDxfId="8"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="outstanding_balance"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="limit" dataDxfId="6">
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="limit" dataDxfId="7">
       <calculatedColumnFormula>Table1[[#This Row],[outstanding_balance]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="baloon"/>
@@ -333,26 +339,29 @@
     <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="contractual_freq"/>
     <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="interest_rate_type"/>
     <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="interest_rate_freq"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="fixed_rate" dataDxfId="5">
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="fixed_rate" dataDxfId="6">
       <calculatedColumnFormula>Table1[[#This Row],[spread]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="spread"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="ltv" dataDxfId="4"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="ltv" dataDxfId="5"/>
     <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="current_arrears"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="contractual_payment" dataDxfId="3">
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="contractual_payment" dataDxfId="4">
       <calculatedColumnFormula>-PMT(M2/K2,DATEDIF(D2,Q2,"y")*I2,E2,-G2,0)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="maturity_date" dataDxfId="2">
       <calculatedColumnFormula>EOMONTH(D2,H2)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="22" xr3:uid="{839146DB-6DF9-42EE-8D52-721111993876}" name="remaining_life" dataDxfId="0">
+      <calculatedColumnFormula>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="collateral_value" dataDxfId="1">
       <calculatedColumnFormula>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="origination_rating"/>
     <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="current_rating">
-      <calculatedColumnFormula>S2</calculatedColumnFormula>
+      <calculatedColumnFormula>T2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="watchlist" dataDxfId="0"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="watchlist" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -621,10 +630,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U121"/>
+  <dimension ref="A1:V121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="U2" sqref="U2"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -642,14 +651,14 @@
     <col min="14" max="14" width="15.140625" customWidth="1"/>
     <col min="15" max="15" width="16.7109375" customWidth="1"/>
     <col min="16" max="16" width="21.85546875" customWidth="1"/>
-    <col min="17" max="17" width="15.7109375" customWidth="1"/>
-    <col min="18" max="18" width="17.28515625" style="2" customWidth="1"/>
-    <col min="19" max="19" width="19" customWidth="1"/>
-    <col min="20" max="20" width="15.7109375" customWidth="1"/>
-    <col min="21" max="21" width="9.140625" style="4"/>
+    <col min="17" max="18" width="15.7109375" customWidth="1"/>
+    <col min="19" max="19" width="17.28515625" style="2" customWidth="1"/>
+    <col min="20" max="20" width="19" customWidth="1"/>
+    <col min="21" max="21" width="15.7109375" customWidth="1"/>
+    <col min="22" max="22" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -701,20 +710,23 @@
       <c r="Q1" t="s">
         <v>7</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="R1" t="s">
+        <v>51</v>
+      </c>
+      <c r="S1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>13</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>14</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="V1" s="4" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43861</v>
       </c>
@@ -771,22 +783,26 @@
         <f t="shared" ref="Q2" si="1">EOMONTH(D2,H2)</f>
         <v>45688</v>
       </c>
-      <c r="R2" s="2">
-        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
-        <v>0</v>
-      </c>
-      <c r="S2">
+      <c r="R2" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>60</v>
+      </c>
+      <c r="S2" s="2">
+        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
         <v>0</v>
       </c>
       <c r="T2">
-        <f t="shared" ref="T2:T12" si="2">S2</f>
-        <v>0</v>
-      </c>
-      <c r="U2" s="4">
+        <v>0</v>
+      </c>
+      <c r="U2">
+        <f t="shared" ref="U2:U12" si="2">T2</f>
+        <v>0</v>
+      </c>
+      <c r="V2" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43861</v>
       </c>
@@ -843,22 +859,26 @@
         <f t="shared" ref="Q3:Q7" si="4">EOMONTH(D3,H3)</f>
         <v>45688</v>
       </c>
-      <c r="R3" s="2">
-        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
-        <v>0</v>
-      </c>
-      <c r="S3">
+      <c r="R3" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>60</v>
+      </c>
+      <c r="S3" s="2">
+        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
         <v>0</v>
       </c>
       <c r="T3">
+        <v>0</v>
+      </c>
+      <c r="U3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U3" s="4">
+      <c r="V3" s="4">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>43861</v>
       </c>
@@ -915,22 +935,26 @@
         <f t="shared" si="4"/>
         <v>44227</v>
       </c>
-      <c r="R4" s="2">
-        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
-        <v>0</v>
-      </c>
-      <c r="S4">
+      <c r="R4" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>12</v>
+      </c>
+      <c r="S4" s="2">
+        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
         <v>0</v>
       </c>
       <c r="T4">
+        <v>0</v>
+      </c>
+      <c r="U4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U4" s="4">
+      <c r="V4" s="4">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>43861</v>
       </c>
@@ -987,19 +1011,23 @@
         <f t="shared" si="4"/>
         <v>45688</v>
       </c>
-      <c r="R5" s="2">
-        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
-        <v>0</v>
-      </c>
-      <c r="S5">
+      <c r="R5" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>60</v>
+      </c>
+      <c r="S5" s="2">
+        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
         <v>0</v>
       </c>
       <c r="T5">
+        <v>0</v>
+      </c>
+      <c r="U5">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>43861</v>
       </c>
@@ -1056,19 +1084,23 @@
         <f t="shared" si="4"/>
         <v>45688</v>
       </c>
-      <c r="R6" s="2">
-        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
-        <v>0</v>
-      </c>
-      <c r="S6">
+      <c r="R6" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>60</v>
+      </c>
+      <c r="S6" s="2">
+        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
         <v>0</v>
       </c>
       <c r="T6">
+        <v>0</v>
+      </c>
+      <c r="U6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>43861</v>
       </c>
@@ -1124,19 +1156,23 @@
         <f t="shared" si="4"/>
         <v>45688</v>
       </c>
-      <c r="R7" s="2">
+      <c r="R7" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>60</v>
+      </c>
+      <c r="S7" s="2">
         <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
         <v>142.85714285714286</v>
       </c>
-      <c r="S7">
-        <v>0</v>
-      </c>
       <c r="T7">
+        <v>0</v>
+      </c>
+      <c r="U7">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>43861</v>
       </c>
@@ -1192,19 +1228,23 @@
         <f t="shared" ref="Q8" si="6">EOMONTH(D8,H8)</f>
         <v>45688</v>
       </c>
-      <c r="R8" s="2">
-        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
-        <v>100</v>
-      </c>
-      <c r="S8">
-        <v>0</v>
+      <c r="R8" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>60</v>
+      </c>
+      <c r="S8" s="2">
+        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
+        <v>100</v>
       </c>
       <c r="T8">
+        <v>0</v>
+      </c>
+      <c r="U8">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>43861</v>
       </c>
@@ -1260,19 +1300,23 @@
         <f t="shared" ref="Q9:Q10" si="8">EOMONTH(D9,H9)</f>
         <v>45688</v>
       </c>
-      <c r="R9" s="2">
+      <c r="R9" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>60</v>
+      </c>
+      <c r="S9" s="2">
         <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
         <v>66.666666666666671</v>
       </c>
-      <c r="S9">
-        <v>0</v>
-      </c>
       <c r="T9">
+        <v>0</v>
+      </c>
+      <c r="U9">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>43861</v>
       </c>
@@ -1329,19 +1373,23 @@
         <f t="shared" si="8"/>
         <v>45688</v>
       </c>
-      <c r="R10" s="2">
-        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
-        <v>0</v>
-      </c>
-      <c r="S10">
+      <c r="R10" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>60</v>
+      </c>
+      <c r="S10" s="2">
+        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
+        <v>0</v>
+      </c>
+      <c r="T10">
         <v>1</v>
       </c>
-      <c r="T10">
+      <c r="U10">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>43861</v>
       </c>
@@ -1398,19 +1446,23 @@
         <f t="shared" ref="Q11" si="10">EOMONTH(D11,H11)</f>
         <v>45688</v>
       </c>
-      <c r="R11" s="2">
-        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
-        <v>0</v>
-      </c>
-      <c r="S11">
+      <c r="R11" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>60</v>
+      </c>
+      <c r="S11" s="2">
+        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
+        <v>0</v>
+      </c>
+      <c r="T11">
         <v>2</v>
       </c>
-      <c r="T11">
+      <c r="U11">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>43861</v>
       </c>
@@ -1467,19 +1519,23 @@
         <f t="shared" ref="Q12:Q13" si="12">EOMONTH(D12,H12)</f>
         <v>45688</v>
       </c>
-      <c r="R12" s="2">
-        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
-        <v>0</v>
-      </c>
-      <c r="S12">
+      <c r="R12" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>60</v>
+      </c>
+      <c r="S12" s="2">
+        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
+        <v>0</v>
+      </c>
+      <c r="T12">
         <v>3</v>
       </c>
-      <c r="T12">
+      <c r="U12">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>43861</v>
       </c>
@@ -1536,18 +1592,22 @@
         <f t="shared" si="12"/>
         <v>45688</v>
       </c>
-      <c r="R13" s="2">
-        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
-        <v>0</v>
-      </c>
-      <c r="S13">
+      <c r="R13" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>60</v>
+      </c>
+      <c r="S13" s="2">
+        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
         <v>0</v>
       </c>
       <c r="T13">
+        <v>0</v>
+      </c>
+      <c r="U13">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>43861</v>
       </c>
@@ -1604,18 +1664,22 @@
         <f t="shared" ref="Q14" si="14">EOMONTH(D14,H14)</f>
         <v>45688</v>
       </c>
-      <c r="R14" s="2">
-        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
-        <v>0</v>
-      </c>
-      <c r="S14">
+      <c r="R14" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>60</v>
+      </c>
+      <c r="S14" s="2">
+        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
         <v>0</v>
       </c>
       <c r="T14">
+        <v>0</v>
+      </c>
+      <c r="U14">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>43861</v>
       </c>
@@ -1672,18 +1736,22 @@
         <f t="shared" ref="Q15" si="16">EOMONTH(D15,H15)</f>
         <v>45688</v>
       </c>
-      <c r="R15" s="2">
-        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
-        <v>0</v>
-      </c>
-      <c r="S15">
+      <c r="R15" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>60</v>
+      </c>
+      <c r="S15" s="2">
+        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
         <v>0</v>
       </c>
       <c r="T15">
+        <v>0</v>
+      </c>
+      <c r="U15">
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>43861</v>
       </c>
@@ -1740,18 +1808,22 @@
         <f t="shared" ref="Q16:Q30" si="18">EOMONTH(D16,H16)</f>
         <v>45688</v>
       </c>
-      <c r="R16" s="2">
-        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
-        <v>0</v>
-      </c>
-      <c r="S16">
+      <c r="R16" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>60</v>
+      </c>
+      <c r="S16" s="2">
+        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
         <v>0</v>
       </c>
       <c r="T16">
+        <v>0</v>
+      </c>
+      <c r="U16">
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>43861</v>
       </c>
@@ -1808,19 +1880,23 @@
         <f t="shared" si="18"/>
         <v>45688</v>
       </c>
-      <c r="R17" s="2">
-        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
-        <v>0</v>
-      </c>
-      <c r="S17">
+      <c r="R17" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>60</v>
+      </c>
+      <c r="S17" s="2">
+        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
         <v>0</v>
       </c>
       <c r="T17">
-        <f t="shared" ref="T17:T27" si="19">S17</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="U17">
+        <f t="shared" ref="U17:U27" si="19">T17</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>43861</v>
       </c>
@@ -1877,19 +1953,23 @@
         <f t="shared" si="18"/>
         <v>45688</v>
       </c>
-      <c r="R18" s="2">
-        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
-        <v>0</v>
-      </c>
-      <c r="S18">
+      <c r="R18" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>60</v>
+      </c>
+      <c r="S18" s="2">
+        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
         <v>0</v>
       </c>
       <c r="T18">
+        <v>0</v>
+      </c>
+      <c r="U18">
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>43861</v>
       </c>
@@ -1946,19 +2026,23 @@
         <f t="shared" si="18"/>
         <v>44227</v>
       </c>
-      <c r="R19" s="2">
-        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
-        <v>0</v>
-      </c>
-      <c r="S19">
+      <c r="R19" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>12</v>
+      </c>
+      <c r="S19" s="2">
+        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
         <v>0</v>
       </c>
       <c r="T19">
+        <v>0</v>
+      </c>
+      <c r="U19">
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>43861</v>
       </c>
@@ -2015,19 +2099,23 @@
         <f t="shared" si="18"/>
         <v>45688</v>
       </c>
-      <c r="R20" s="2">
-        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
-        <v>0</v>
-      </c>
-      <c r="S20">
+      <c r="R20" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>60</v>
+      </c>
+      <c r="S20" s="2">
+        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
         <v>0</v>
       </c>
       <c r="T20">
+        <v>0</v>
+      </c>
+      <c r="U20">
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>43861</v>
       </c>
@@ -2084,19 +2172,23 @@
         <f t="shared" si="18"/>
         <v>45688</v>
       </c>
-      <c r="R21" s="2">
-        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
-        <v>0</v>
-      </c>
-      <c r="S21">
+      <c r="R21" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>60</v>
+      </c>
+      <c r="S21" s="2">
+        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
         <v>0</v>
       </c>
       <c r="T21">
+        <v>0</v>
+      </c>
+      <c r="U21">
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>43861</v>
       </c>
@@ -2152,19 +2244,23 @@
         <f t="shared" si="18"/>
         <v>45688</v>
       </c>
-      <c r="R22" s="2">
+      <c r="R22" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>60</v>
+      </c>
+      <c r="S22" s="2">
         <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
         <v>142.85714285714286</v>
       </c>
-      <c r="S22">
-        <v>0</v>
-      </c>
       <c r="T22">
+        <v>0</v>
+      </c>
+      <c r="U22">
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>43861</v>
       </c>
@@ -2220,19 +2316,23 @@
         <f t="shared" si="18"/>
         <v>45688</v>
       </c>
-      <c r="R23" s="2">
-        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
-        <v>100</v>
-      </c>
-      <c r="S23">
-        <v>0</v>
+      <c r="R23" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>60</v>
+      </c>
+      <c r="S23" s="2">
+        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
+        <v>100</v>
       </c>
       <c r="T23">
+        <v>0</v>
+      </c>
+      <c r="U23">
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>43861</v>
       </c>
@@ -2288,19 +2388,23 @@
         <f t="shared" si="18"/>
         <v>45688</v>
       </c>
-      <c r="R24" s="2">
+      <c r="R24" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>60</v>
+      </c>
+      <c r="S24" s="2">
         <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
         <v>66.666666666666671</v>
       </c>
-      <c r="S24">
-        <v>0</v>
-      </c>
       <c r="T24">
+        <v>0</v>
+      </c>
+      <c r="U24">
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>43861</v>
       </c>
@@ -2357,19 +2461,23 @@
         <f t="shared" si="18"/>
         <v>45688</v>
       </c>
-      <c r="R25" s="2">
-        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
-        <v>0</v>
-      </c>
-      <c r="S25">
+      <c r="R25" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>60</v>
+      </c>
+      <c r="S25" s="2">
+        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
+        <v>0</v>
+      </c>
+      <c r="T25">
         <v>1</v>
       </c>
-      <c r="T25">
+      <c r="U25">
         <f t="shared" si="19"/>
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>43861</v>
       </c>
@@ -2426,19 +2534,23 @@
         <f t="shared" si="18"/>
         <v>45688</v>
       </c>
-      <c r="R26" s="2">
-        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
-        <v>0</v>
-      </c>
-      <c r="S26">
+      <c r="R26" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>60</v>
+      </c>
+      <c r="S26" s="2">
+        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
+        <v>0</v>
+      </c>
+      <c r="T26">
         <v>2</v>
       </c>
-      <c r="T26">
+      <c r="U26">
         <f t="shared" si="19"/>
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>43861</v>
       </c>
@@ -2495,19 +2607,23 @@
         <f t="shared" si="18"/>
         <v>45688</v>
       </c>
-      <c r="R27" s="2">
-        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
-        <v>0</v>
-      </c>
-      <c r="S27">
+      <c r="R27" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>60</v>
+      </c>
+      <c r="S27" s="2">
+        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
+        <v>0</v>
+      </c>
+      <c r="T27">
         <v>3</v>
       </c>
-      <c r="T27">
+      <c r="U27">
         <f t="shared" si="19"/>
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>43861</v>
       </c>
@@ -2564,18 +2680,22 @@
         <f t="shared" si="18"/>
         <v>45688</v>
       </c>
-      <c r="R28" s="2">
-        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
-        <v>0</v>
-      </c>
-      <c r="S28">
+      <c r="R28" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>60</v>
+      </c>
+      <c r="S28" s="2">
+        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
         <v>0</v>
       </c>
       <c r="T28">
+        <v>0</v>
+      </c>
+      <c r="U28">
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>43861</v>
       </c>
@@ -2632,18 +2752,22 @@
         <f t="shared" si="18"/>
         <v>45688</v>
       </c>
-      <c r="R29" s="2">
-        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
-        <v>0</v>
-      </c>
-      <c r="S29">
+      <c r="R29" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>60</v>
+      </c>
+      <c r="S29" s="2">
+        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
         <v>0</v>
       </c>
       <c r="T29">
+        <v>0</v>
+      </c>
+      <c r="U29">
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>43861</v>
       </c>
@@ -2700,18 +2824,22 @@
         <f t="shared" si="18"/>
         <v>45688</v>
       </c>
-      <c r="R30" s="2">
-        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
-        <v>0</v>
-      </c>
-      <c r="S30">
+      <c r="R30" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>60</v>
+      </c>
+      <c r="S30" s="2">
+        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
         <v>0</v>
       </c>
       <c r="T30">
+        <v>0</v>
+      </c>
+      <c r="U30">
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>43861</v>
       </c>
@@ -2768,18 +2896,22 @@
         <f t="shared" ref="Q31:Q45" si="21">EOMONTH(D31,H31)</f>
         <v>45688</v>
       </c>
-      <c r="R31" s="2">
-        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
-        <v>0</v>
-      </c>
-      <c r="S31">
+      <c r="R31" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>60</v>
+      </c>
+      <c r="S31" s="2">
+        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
         <v>0</v>
       </c>
       <c r="T31">
+        <v>0</v>
+      </c>
+      <c r="U31">
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>43861</v>
       </c>
@@ -2836,19 +2968,23 @@
         <f t="shared" si="21"/>
         <v>45688</v>
       </c>
-      <c r="R32" s="2">
-        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
-        <v>0</v>
-      </c>
-      <c r="S32">
+      <c r="R32" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>60</v>
+      </c>
+      <c r="S32" s="2">
+        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
         <v>0</v>
       </c>
       <c r="T32">
-        <f t="shared" ref="T32:T42" si="22">S32</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="U32">
+        <f t="shared" ref="U32:U42" si="22">T32</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>43861</v>
       </c>
@@ -2905,19 +3041,23 @@
         <f t="shared" si="21"/>
         <v>45688</v>
       </c>
-      <c r="R33" s="2">
-        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
-        <v>0</v>
-      </c>
-      <c r="S33">
+      <c r="R33" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>60</v>
+      </c>
+      <c r="S33" s="2">
+        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
         <v>0</v>
       </c>
       <c r="T33">
+        <v>0</v>
+      </c>
+      <c r="U33">
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>43861</v>
       </c>
@@ -2974,19 +3114,23 @@
         <f t="shared" si="21"/>
         <v>44227</v>
       </c>
-      <c r="R34" s="2">
-        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
-        <v>0</v>
-      </c>
-      <c r="S34">
+      <c r="R34" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>12</v>
+      </c>
+      <c r="S34" s="2">
+        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
         <v>0</v>
       </c>
       <c r="T34">
+        <v>0</v>
+      </c>
+      <c r="U34">
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>43861</v>
       </c>
@@ -3043,19 +3187,23 @@
         <f t="shared" si="21"/>
         <v>45688</v>
       </c>
-      <c r="R35" s="2">
-        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
-        <v>0</v>
-      </c>
-      <c r="S35">
+      <c r="R35" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>60</v>
+      </c>
+      <c r="S35" s="2">
+        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
         <v>0</v>
       </c>
       <c r="T35">
+        <v>0</v>
+      </c>
+      <c r="U35">
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>43861</v>
       </c>
@@ -3112,19 +3260,23 @@
         <f t="shared" si="21"/>
         <v>45688</v>
       </c>
-      <c r="R36" s="2">
-        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
-        <v>0</v>
-      </c>
-      <c r="S36">
+      <c r="R36" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>60</v>
+      </c>
+      <c r="S36" s="2">
+        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
         <v>0</v>
       </c>
       <c r="T36">
+        <v>0</v>
+      </c>
+      <c r="U36">
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>43861</v>
       </c>
@@ -3180,19 +3332,23 @@
         <f t="shared" si="21"/>
         <v>45688</v>
       </c>
-      <c r="R37" s="2">
+      <c r="R37" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>60</v>
+      </c>
+      <c r="S37" s="2">
         <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
         <v>142.85714285714286</v>
       </c>
-      <c r="S37">
-        <v>0</v>
-      </c>
       <c r="T37">
+        <v>0</v>
+      </c>
+      <c r="U37">
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>43861</v>
       </c>
@@ -3248,19 +3404,23 @@
         <f t="shared" si="21"/>
         <v>45688</v>
       </c>
-      <c r="R38" s="2">
-        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
-        <v>100</v>
-      </c>
-      <c r="S38">
-        <v>0</v>
+      <c r="R38" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>60</v>
+      </c>
+      <c r="S38" s="2">
+        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
+        <v>100</v>
       </c>
       <c r="T38">
+        <v>0</v>
+      </c>
+      <c r="U38">
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>43861</v>
       </c>
@@ -3316,19 +3476,23 @@
         <f t="shared" si="21"/>
         <v>45688</v>
       </c>
-      <c r="R39" s="2">
+      <c r="R39" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>60</v>
+      </c>
+      <c r="S39" s="2">
         <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
         <v>66.666666666666671</v>
       </c>
-      <c r="S39">
-        <v>0</v>
-      </c>
       <c r="T39">
+        <v>0</v>
+      </c>
+      <c r="U39">
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>43861</v>
       </c>
@@ -3385,19 +3549,23 @@
         <f t="shared" si="21"/>
         <v>45688</v>
       </c>
-      <c r="R40" s="2">
-        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
-        <v>0</v>
-      </c>
-      <c r="S40">
+      <c r="R40" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>60</v>
+      </c>
+      <c r="S40" s="2">
+        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
+        <v>0</v>
+      </c>
+      <c r="T40">
         <v>1</v>
       </c>
-      <c r="T40">
+      <c r="U40">
         <f t="shared" si="22"/>
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>43861</v>
       </c>
@@ -3454,19 +3622,23 @@
         <f t="shared" si="21"/>
         <v>45688</v>
       </c>
-      <c r="R41" s="2">
-        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
-        <v>0</v>
-      </c>
-      <c r="S41">
+      <c r="R41" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>60</v>
+      </c>
+      <c r="S41" s="2">
+        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
+        <v>0</v>
+      </c>
+      <c r="T41">
         <v>2</v>
       </c>
-      <c r="T41">
+      <c r="U41">
         <f t="shared" si="22"/>
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>43861</v>
       </c>
@@ -3523,19 +3695,23 @@
         <f t="shared" si="21"/>
         <v>45688</v>
       </c>
-      <c r="R42" s="2">
-        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
-        <v>0</v>
-      </c>
-      <c r="S42">
+      <c r="R42" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>60</v>
+      </c>
+      <c r="S42" s="2">
+        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
+        <v>0</v>
+      </c>
+      <c r="T42">
         <v>3</v>
       </c>
-      <c r="T42">
+      <c r="U42">
         <f t="shared" si="22"/>
         <v>3</v>
       </c>
     </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>43861</v>
       </c>
@@ -3592,18 +3768,22 @@
         <f t="shared" si="21"/>
         <v>45688</v>
       </c>
-      <c r="R43" s="2">
-        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
-        <v>0</v>
-      </c>
-      <c r="S43">
+      <c r="R43" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>60</v>
+      </c>
+      <c r="S43" s="2">
+        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
         <v>0</v>
       </c>
       <c r="T43">
+        <v>0</v>
+      </c>
+      <c r="U43">
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>43861</v>
       </c>
@@ -3660,18 +3840,22 @@
         <f t="shared" si="21"/>
         <v>45688</v>
       </c>
-      <c r="R44" s="2">
-        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
-        <v>0</v>
-      </c>
-      <c r="S44">
+      <c r="R44" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>60</v>
+      </c>
+      <c r="S44" s="2">
+        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
         <v>0</v>
       </c>
       <c r="T44">
+        <v>0</v>
+      </c>
+      <c r="U44">
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>43861</v>
       </c>
@@ -3728,18 +3912,22 @@
         <f t="shared" si="21"/>
         <v>45688</v>
       </c>
-      <c r="R45" s="2">
-        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
-        <v>0</v>
-      </c>
-      <c r="S45">
+      <c r="R45" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>60</v>
+      </c>
+      <c r="S45" s="2">
+        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
         <v>0</v>
       </c>
       <c r="T45">
+        <v>0</v>
+      </c>
+      <c r="U45">
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>43861</v>
       </c>
@@ -3796,18 +3984,22 @@
         <f t="shared" ref="Q46:Q60" si="24">EOMONTH(D46,H46)</f>
         <v>45688</v>
       </c>
-      <c r="R46" s="2">
-        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
-        <v>0</v>
-      </c>
-      <c r="S46">
+      <c r="R46" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>60</v>
+      </c>
+      <c r="S46" s="2">
+        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
         <v>0</v>
       </c>
       <c r="T46">
+        <v>0</v>
+      </c>
+      <c r="U46">
         <v>4</v>
       </c>
     </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>43861</v>
       </c>
@@ -3864,19 +4056,23 @@
         <f t="shared" si="24"/>
         <v>45688</v>
       </c>
-      <c r="R47" s="2">
-        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
-        <v>0</v>
-      </c>
-      <c r="S47">
+      <c r="R47" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>60</v>
+      </c>
+      <c r="S47" s="2">
+        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
         <v>0</v>
       </c>
       <c r="T47">
-        <f t="shared" ref="T47:T57" si="25">S47</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="U47">
+        <f t="shared" ref="U47:U57" si="25">T47</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>43861</v>
       </c>
@@ -3933,19 +4129,23 @@
         <f t="shared" si="24"/>
         <v>45688</v>
       </c>
-      <c r="R48" s="2">
-        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
-        <v>0</v>
-      </c>
-      <c r="S48">
+      <c r="R48" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>60</v>
+      </c>
+      <c r="S48" s="2">
+        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
         <v>0</v>
       </c>
       <c r="T48">
+        <v>0</v>
+      </c>
+      <c r="U48">
         <f t="shared" si="25"/>
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>43861</v>
       </c>
@@ -4002,19 +4202,23 @@
         <f t="shared" si="24"/>
         <v>44227</v>
       </c>
-      <c r="R49" s="2">
-        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
-        <v>0</v>
-      </c>
-      <c r="S49">
+      <c r="R49" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>12</v>
+      </c>
+      <c r="S49" s="2">
+        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
         <v>0</v>
       </c>
       <c r="T49">
+        <v>0</v>
+      </c>
+      <c r="U49">
         <f t="shared" si="25"/>
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>43861</v>
       </c>
@@ -4071,19 +4275,23 @@
         <f t="shared" si="24"/>
         <v>45688</v>
       </c>
-      <c r="R50" s="2">
-        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
-        <v>0</v>
-      </c>
-      <c r="S50">
+      <c r="R50" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>60</v>
+      </c>
+      <c r="S50" s="2">
+        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
         <v>0</v>
       </c>
       <c r="T50">
+        <v>0</v>
+      </c>
+      <c r="U50">
         <f t="shared" si="25"/>
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>43861</v>
       </c>
@@ -4140,19 +4348,23 @@
         <f t="shared" si="24"/>
         <v>45688</v>
       </c>
-      <c r="R51" s="2">
-        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
-        <v>0</v>
-      </c>
-      <c r="S51">
+      <c r="R51" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>60</v>
+      </c>
+      <c r="S51" s="2">
+        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
         <v>0</v>
       </c>
       <c r="T51">
+        <v>0</v>
+      </c>
+      <c r="U51">
         <f t="shared" si="25"/>
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>43861</v>
       </c>
@@ -4208,19 +4420,23 @@
         <f t="shared" si="24"/>
         <v>45688</v>
       </c>
-      <c r="R52" s="2">
+      <c r="R52" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>60</v>
+      </c>
+      <c r="S52" s="2">
         <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
         <v>142.85714285714286</v>
       </c>
-      <c r="S52">
-        <v>0</v>
-      </c>
       <c r="T52">
+        <v>0</v>
+      </c>
+      <c r="U52">
         <f t="shared" si="25"/>
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>43861</v>
       </c>
@@ -4276,19 +4492,23 @@
         <f t="shared" si="24"/>
         <v>45688</v>
       </c>
-      <c r="R53" s="2">
-        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
-        <v>100</v>
-      </c>
-      <c r="S53">
-        <v>0</v>
+      <c r="R53" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>60</v>
+      </c>
+      <c r="S53" s="2">
+        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
+        <v>100</v>
       </c>
       <c r="T53">
+        <v>0</v>
+      </c>
+      <c r="U53">
         <f t="shared" si="25"/>
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>43861</v>
       </c>
@@ -4344,19 +4564,23 @@
         <f t="shared" si="24"/>
         <v>45688</v>
       </c>
-      <c r="R54" s="2">
+      <c r="R54" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>60</v>
+      </c>
+      <c r="S54" s="2">
         <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
         <v>66.666666666666671</v>
       </c>
-      <c r="S54">
-        <v>0</v>
-      </c>
       <c r="T54">
+        <v>0</v>
+      </c>
+      <c r="U54">
         <f t="shared" si="25"/>
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>43861</v>
       </c>
@@ -4413,19 +4637,23 @@
         <f t="shared" si="24"/>
         <v>45688</v>
       </c>
-      <c r="R55" s="2">
-        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
-        <v>0</v>
-      </c>
-      <c r="S55">
+      <c r="R55" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>60</v>
+      </c>
+      <c r="S55" s="2">
+        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
+        <v>0</v>
+      </c>
+      <c r="T55">
         <v>1</v>
       </c>
-      <c r="T55">
+      <c r="U55">
         <f t="shared" si="25"/>
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>43861</v>
       </c>
@@ -4482,19 +4710,23 @@
         <f t="shared" si="24"/>
         <v>45688</v>
       </c>
-      <c r="R56" s="2">
-        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
-        <v>0</v>
-      </c>
-      <c r="S56">
+      <c r="R56" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>60</v>
+      </c>
+      <c r="S56" s="2">
+        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
+        <v>0</v>
+      </c>
+      <c r="T56">
         <v>2</v>
       </c>
-      <c r="T56">
+      <c r="U56">
         <f t="shared" si="25"/>
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>43861</v>
       </c>
@@ -4551,19 +4783,23 @@
         <f t="shared" si="24"/>
         <v>45688</v>
       </c>
-      <c r="R57" s="2">
-        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
-        <v>0</v>
-      </c>
-      <c r="S57">
+      <c r="R57" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>60</v>
+      </c>
+      <c r="S57" s="2">
+        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
+        <v>0</v>
+      </c>
+      <c r="T57">
         <v>3</v>
       </c>
-      <c r="T57">
+      <c r="U57">
         <f t="shared" si="25"/>
         <v>3</v>
       </c>
     </row>
-    <row r="58" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>43861</v>
       </c>
@@ -4620,18 +4856,22 @@
         <f t="shared" si="24"/>
         <v>45688</v>
       </c>
-      <c r="R58" s="2">
-        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
-        <v>0</v>
-      </c>
-      <c r="S58">
+      <c r="R58" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>60</v>
+      </c>
+      <c r="S58" s="2">
+        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
         <v>0</v>
       </c>
       <c r="T58">
+        <v>0</v>
+      </c>
+      <c r="U58">
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>43861</v>
       </c>
@@ -4688,18 +4928,22 @@
         <f t="shared" si="24"/>
         <v>45688</v>
       </c>
-      <c r="R59" s="2">
-        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
-        <v>0</v>
-      </c>
-      <c r="S59">
+      <c r="R59" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>60</v>
+      </c>
+      <c r="S59" s="2">
+        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
         <v>0</v>
       </c>
       <c r="T59">
+        <v>0</v>
+      </c>
+      <c r="U59">
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>43861</v>
       </c>
@@ -4756,18 +5000,22 @@
         <f t="shared" si="24"/>
         <v>45688</v>
       </c>
-      <c r="R60" s="2">
-        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
-        <v>0</v>
-      </c>
-      <c r="S60">
+      <c r="R60" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>60</v>
+      </c>
+      <c r="S60" s="2">
+        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
         <v>0</v>
       </c>
       <c r="T60">
+        <v>0</v>
+      </c>
+      <c r="U60">
         <v>3</v>
       </c>
     </row>
-    <row r="61" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>43861</v>
       </c>
@@ -4824,18 +5072,22 @@
         <f t="shared" ref="Q61:Q120" si="27">EOMONTH(D61,H61)</f>
         <v>45688</v>
       </c>
-      <c r="R61" s="2">
-        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
-        <v>0</v>
-      </c>
-      <c r="S61">
+      <c r="R61" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>60</v>
+      </c>
+      <c r="S61" s="2">
+        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
         <v>0</v>
       </c>
       <c r="T61">
+        <v>0</v>
+      </c>
+      <c r="U61">
         <v>4</v>
       </c>
     </row>
-    <row r="62" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>44227</v>
       </c>
@@ -4892,19 +5144,23 @@
         <f t="shared" si="27"/>
         <v>46053</v>
       </c>
-      <c r="R62" s="2">
-        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
-        <v>0</v>
-      </c>
-      <c r="S62">
+      <c r="R62" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>60</v>
+      </c>
+      <c r="S62" s="2">
+        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
         <v>0</v>
       </c>
       <c r="T62">
-        <f t="shared" ref="T62:T72" si="28">S62</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:20" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="U62">
+        <f t="shared" ref="U62:U72" si="28">T62</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>44227</v>
       </c>
@@ -4961,19 +5217,23 @@
         <f t="shared" si="27"/>
         <v>46053</v>
       </c>
-      <c r="R63" s="2">
-        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
-        <v>0</v>
-      </c>
-      <c r="S63">
+      <c r="R63" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>60</v>
+      </c>
+      <c r="S63" s="2">
+        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
         <v>0</v>
       </c>
       <c r="T63">
+        <v>0</v>
+      </c>
+      <c r="U63">
         <f t="shared" si="28"/>
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>44227</v>
       </c>
@@ -5030,19 +5290,23 @@
         <f t="shared" si="27"/>
         <v>44592</v>
       </c>
-      <c r="R64" s="2">
-        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
-        <v>0</v>
-      </c>
-      <c r="S64">
+      <c r="R64" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>12</v>
+      </c>
+      <c r="S64" s="2">
+        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
         <v>0</v>
       </c>
       <c r="T64">
+        <v>0</v>
+      </c>
+      <c r="U64">
         <f t="shared" si="28"/>
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>44227</v>
       </c>
@@ -5099,19 +5363,23 @@
         <f t="shared" si="27"/>
         <v>46053</v>
       </c>
-      <c r="R65" s="2">
-        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
-        <v>0</v>
-      </c>
-      <c r="S65">
+      <c r="R65" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>60</v>
+      </c>
+      <c r="S65" s="2">
+        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
         <v>0</v>
       </c>
       <c r="T65">
+        <v>0</v>
+      </c>
+      <c r="U65">
         <f t="shared" si="28"/>
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>44227</v>
       </c>
@@ -5168,19 +5436,23 @@
         <f t="shared" si="27"/>
         <v>46053</v>
       </c>
-      <c r="R66" s="2">
-        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
-        <v>0</v>
-      </c>
-      <c r="S66">
+      <c r="R66" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>60</v>
+      </c>
+      <c r="S66" s="2">
+        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
         <v>0</v>
       </c>
       <c r="T66">
+        <v>0</v>
+      </c>
+      <c r="U66">
         <f t="shared" si="28"/>
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>44227</v>
       </c>
@@ -5236,19 +5508,23 @@
         <f t="shared" si="27"/>
         <v>46053</v>
       </c>
-      <c r="R67" s="2">
+      <c r="R67" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>60</v>
+      </c>
+      <c r="S67" s="2">
         <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
         <v>142.85714285714286</v>
       </c>
-      <c r="S67">
-        <v>0</v>
-      </c>
       <c r="T67">
+        <v>0</v>
+      </c>
+      <c r="U67">
         <f t="shared" si="28"/>
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>44227</v>
       </c>
@@ -5304,19 +5580,23 @@
         <f t="shared" si="27"/>
         <v>46053</v>
       </c>
-      <c r="R68" s="2">
-        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
-        <v>100</v>
-      </c>
-      <c r="S68">
-        <v>0</v>
+      <c r="R68" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>60</v>
+      </c>
+      <c r="S68" s="2">
+        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
+        <v>100</v>
       </c>
       <c r="T68">
+        <v>0</v>
+      </c>
+      <c r="U68">
         <f t="shared" si="28"/>
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>44227</v>
       </c>
@@ -5372,19 +5652,23 @@
         <f t="shared" si="27"/>
         <v>46053</v>
       </c>
-      <c r="R69" s="2">
+      <c r="R69" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>60</v>
+      </c>
+      <c r="S69" s="2">
         <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
         <v>66.666666666666671</v>
       </c>
-      <c r="S69">
-        <v>0</v>
-      </c>
       <c r="T69">
+        <v>0</v>
+      </c>
+      <c r="U69">
         <f t="shared" si="28"/>
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>44227</v>
       </c>
@@ -5441,19 +5725,23 @@
         <f t="shared" si="27"/>
         <v>46053</v>
       </c>
-      <c r="R70" s="2">
-        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
-        <v>0</v>
-      </c>
-      <c r="S70">
+      <c r="R70" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>60</v>
+      </c>
+      <c r="S70" s="2">
+        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
+        <v>0</v>
+      </c>
+      <c r="T70">
         <v>1</v>
       </c>
-      <c r="T70">
+      <c r="U70">
         <f t="shared" si="28"/>
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>44227</v>
       </c>
@@ -5510,19 +5798,23 @@
         <f t="shared" si="27"/>
         <v>46053</v>
       </c>
-      <c r="R71" s="2">
-        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
-        <v>0</v>
-      </c>
-      <c r="S71">
+      <c r="R71" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>60</v>
+      </c>
+      <c r="S71" s="2">
+        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
+        <v>0</v>
+      </c>
+      <c r="T71">
         <v>2</v>
       </c>
-      <c r="T71">
+      <c r="U71">
         <f t="shared" si="28"/>
         <v>2</v>
       </c>
     </row>
-    <row r="72" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>44227</v>
       </c>
@@ -5579,19 +5871,23 @@
         <f t="shared" si="27"/>
         <v>46053</v>
       </c>
-      <c r="R72" s="2">
-        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
-        <v>0</v>
-      </c>
-      <c r="S72">
+      <c r="R72" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>60</v>
+      </c>
+      <c r="S72" s="2">
+        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
+        <v>0</v>
+      </c>
+      <c r="T72">
         <v>3</v>
       </c>
-      <c r="T72">
+      <c r="U72">
         <f t="shared" si="28"/>
         <v>3</v>
       </c>
     </row>
-    <row r="73" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>44227</v>
       </c>
@@ -5648,18 +5944,22 @@
         <f t="shared" si="27"/>
         <v>46053</v>
       </c>
-      <c r="R73" s="2">
-        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
-        <v>0</v>
-      </c>
-      <c r="S73">
+      <c r="R73" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>60</v>
+      </c>
+      <c r="S73" s="2">
+        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
         <v>0</v>
       </c>
       <c r="T73">
+        <v>0</v>
+      </c>
+      <c r="U73">
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>44227</v>
       </c>
@@ -5716,18 +6016,22 @@
         <f t="shared" si="27"/>
         <v>46053</v>
       </c>
-      <c r="R74" s="2">
-        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
-        <v>0</v>
-      </c>
-      <c r="S74">
+      <c r="R74" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>60</v>
+      </c>
+      <c r="S74" s="2">
+        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
         <v>0</v>
       </c>
       <c r="T74">
+        <v>0</v>
+      </c>
+      <c r="U74">
         <v>2</v>
       </c>
     </row>
-    <row r="75" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>44227</v>
       </c>
@@ -5784,18 +6088,22 @@
         <f t="shared" si="27"/>
         <v>46053</v>
       </c>
-      <c r="R75" s="2">
-        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
-        <v>0</v>
-      </c>
-      <c r="S75">
+      <c r="R75" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>60</v>
+      </c>
+      <c r="S75" s="2">
+        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
         <v>0</v>
       </c>
       <c r="T75">
+        <v>0</v>
+      </c>
+      <c r="U75">
         <v>3</v>
       </c>
     </row>
-    <row r="76" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>44227</v>
       </c>
@@ -5852,18 +6160,22 @@
         <f t="shared" si="27"/>
         <v>46053</v>
       </c>
-      <c r="R76" s="2">
-        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
-        <v>0</v>
-      </c>
-      <c r="S76">
+      <c r="R76" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>60</v>
+      </c>
+      <c r="S76" s="2">
+        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
         <v>0</v>
       </c>
       <c r="T76">
+        <v>0</v>
+      </c>
+      <c r="U76">
         <v>4</v>
       </c>
     </row>
-    <row r="77" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>44227</v>
       </c>
@@ -5920,19 +6232,23 @@
         <f t="shared" si="27"/>
         <v>46053</v>
       </c>
-      <c r="R77" s="2">
-        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
-        <v>0</v>
-      </c>
-      <c r="S77">
+      <c r="R77" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>60</v>
+      </c>
+      <c r="S77" s="2">
+        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
         <v>0</v>
       </c>
       <c r="T77">
-        <f t="shared" ref="T77:T87" si="29">S77</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="78" spans="1:20" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="U77">
+        <f t="shared" ref="U77:U87" si="29">T77</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>44227</v>
       </c>
@@ -5989,19 +6305,23 @@
         <f t="shared" si="27"/>
         <v>46053</v>
       </c>
-      <c r="R78" s="2">
-        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
-        <v>0</v>
-      </c>
-      <c r="S78">
+      <c r="R78" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>60</v>
+      </c>
+      <c r="S78" s="2">
+        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
         <v>0</v>
       </c>
       <c r="T78">
+        <v>0</v>
+      </c>
+      <c r="U78">
         <f t="shared" si="29"/>
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>44227</v>
       </c>
@@ -6058,19 +6378,23 @@
         <f t="shared" si="27"/>
         <v>44592</v>
       </c>
-      <c r="R79" s="2">
-        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
-        <v>0</v>
-      </c>
-      <c r="S79">
+      <c r="R79" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>12</v>
+      </c>
+      <c r="S79" s="2">
+        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
         <v>0</v>
       </c>
       <c r="T79">
+        <v>0</v>
+      </c>
+      <c r="U79">
         <f t="shared" si="29"/>
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>44227</v>
       </c>
@@ -6127,19 +6451,23 @@
         <f t="shared" si="27"/>
         <v>46053</v>
       </c>
-      <c r="R80" s="2">
-        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
-        <v>0</v>
-      </c>
-      <c r="S80">
+      <c r="R80" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>60</v>
+      </c>
+      <c r="S80" s="2">
+        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
         <v>0</v>
       </c>
       <c r="T80">
+        <v>0</v>
+      </c>
+      <c r="U80">
         <f t="shared" si="29"/>
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>44227</v>
       </c>
@@ -6196,19 +6524,23 @@
         <f t="shared" si="27"/>
         <v>46053</v>
       </c>
-      <c r="R81" s="2">
-        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
-        <v>0</v>
-      </c>
-      <c r="S81">
+      <c r="R81" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>60</v>
+      </c>
+      <c r="S81" s="2">
+        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
         <v>0</v>
       </c>
       <c r="T81">
+        <v>0</v>
+      </c>
+      <c r="U81">
         <f t="shared" si="29"/>
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>44227</v>
       </c>
@@ -6264,19 +6596,23 @@
         <f t="shared" si="27"/>
         <v>46053</v>
       </c>
-      <c r="R82" s="2">
+      <c r="R82" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>60</v>
+      </c>
+      <c r="S82" s="2">
         <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
         <v>142.85714285714286</v>
       </c>
-      <c r="S82">
-        <v>0</v>
-      </c>
       <c r="T82">
+        <v>0</v>
+      </c>
+      <c r="U82">
         <f t="shared" si="29"/>
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>44227</v>
       </c>
@@ -6332,19 +6668,23 @@
         <f t="shared" si="27"/>
         <v>46053</v>
       </c>
-      <c r="R83" s="2">
-        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
-        <v>100</v>
-      </c>
-      <c r="S83">
-        <v>0</v>
+      <c r="R83" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>60</v>
+      </c>
+      <c r="S83" s="2">
+        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
+        <v>100</v>
       </c>
       <c r="T83">
+        <v>0</v>
+      </c>
+      <c r="U83">
         <f t="shared" si="29"/>
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>44227</v>
       </c>
@@ -6400,19 +6740,23 @@
         <f t="shared" si="27"/>
         <v>46053</v>
       </c>
-      <c r="R84" s="2">
+      <c r="R84" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>60</v>
+      </c>
+      <c r="S84" s="2">
         <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
         <v>66.666666666666671</v>
       </c>
-      <c r="S84">
-        <v>0</v>
-      </c>
       <c r="T84">
+        <v>0</v>
+      </c>
+      <c r="U84">
         <f t="shared" si="29"/>
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>44227</v>
       </c>
@@ -6469,19 +6813,23 @@
         <f t="shared" si="27"/>
         <v>46053</v>
       </c>
-      <c r="R85" s="2">
-        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
-        <v>0</v>
-      </c>
-      <c r="S85">
+      <c r="R85" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>60</v>
+      </c>
+      <c r="S85" s="2">
+        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
+        <v>0</v>
+      </c>
+      <c r="T85">
         <v>1</v>
       </c>
-      <c r="T85">
+      <c r="U85">
         <f t="shared" si="29"/>
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>44227</v>
       </c>
@@ -6538,19 +6886,23 @@
         <f t="shared" si="27"/>
         <v>46053</v>
       </c>
-      <c r="R86" s="2">
-        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
-        <v>0</v>
-      </c>
-      <c r="S86">
+      <c r="R86" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>60</v>
+      </c>
+      <c r="S86" s="2">
+        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
+        <v>0</v>
+      </c>
+      <c r="T86">
         <v>2</v>
       </c>
-      <c r="T86">
+      <c r="U86">
         <f t="shared" si="29"/>
         <v>2</v>
       </c>
     </row>
-    <row r="87" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>44227</v>
       </c>
@@ -6607,19 +6959,23 @@
         <f t="shared" si="27"/>
         <v>46053</v>
       </c>
-      <c r="R87" s="2">
-        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
-        <v>0</v>
-      </c>
-      <c r="S87">
+      <c r="R87" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>60</v>
+      </c>
+      <c r="S87" s="2">
+        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
+        <v>0</v>
+      </c>
+      <c r="T87">
         <v>3</v>
       </c>
-      <c r="T87">
+      <c r="U87">
         <f t="shared" si="29"/>
         <v>3</v>
       </c>
     </row>
-    <row r="88" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>44227</v>
       </c>
@@ -6676,18 +7032,22 @@
         <f t="shared" si="27"/>
         <v>46053</v>
       </c>
-      <c r="R88" s="2">
-        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
-        <v>0</v>
-      </c>
-      <c r="S88">
+      <c r="R88" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>60</v>
+      </c>
+      <c r="S88" s="2">
+        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
         <v>0</v>
       </c>
       <c r="T88">
+        <v>0</v>
+      </c>
+      <c r="U88">
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>44227</v>
       </c>
@@ -6744,18 +7104,22 @@
         <f t="shared" si="27"/>
         <v>46053</v>
       </c>
-      <c r="R89" s="2">
-        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
-        <v>0</v>
-      </c>
-      <c r="S89">
+      <c r="R89" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>60</v>
+      </c>
+      <c r="S89" s="2">
+        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
         <v>0</v>
       </c>
       <c r="T89">
+        <v>0</v>
+      </c>
+      <c r="U89">
         <v>2</v>
       </c>
     </row>
-    <row r="90" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>44227</v>
       </c>
@@ -6812,18 +7176,22 @@
         <f t="shared" si="27"/>
         <v>46053</v>
       </c>
-      <c r="R90" s="2">
-        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
-        <v>0</v>
-      </c>
-      <c r="S90">
+      <c r="R90" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>60</v>
+      </c>
+      <c r="S90" s="2">
+        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
         <v>0</v>
       </c>
       <c r="T90">
+        <v>0</v>
+      </c>
+      <c r="U90">
         <v>3</v>
       </c>
     </row>
-    <row r="91" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>44227</v>
       </c>
@@ -6880,18 +7248,22 @@
         <f t="shared" si="27"/>
         <v>46053</v>
       </c>
-      <c r="R91" s="2">
-        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
-        <v>0</v>
-      </c>
-      <c r="S91">
+      <c r="R91" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>60</v>
+      </c>
+      <c r="S91" s="2">
+        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
         <v>0</v>
       </c>
       <c r="T91">
+        <v>0</v>
+      </c>
+      <c r="U91">
         <v>4</v>
       </c>
     </row>
-    <row r="92" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>44227</v>
       </c>
@@ -6948,19 +7320,23 @@
         <f t="shared" si="27"/>
         <v>46053</v>
       </c>
-      <c r="R92" s="2">
-        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
-        <v>0</v>
-      </c>
-      <c r="S92">
+      <c r="R92" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>60</v>
+      </c>
+      <c r="S92" s="2">
+        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
         <v>0</v>
       </c>
       <c r="T92">
-        <f t="shared" ref="T92:T102" si="30">S92</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="93" spans="1:20" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="U92">
+        <f t="shared" ref="U92:U102" si="30">T92</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>44227</v>
       </c>
@@ -7017,19 +7393,23 @@
         <f t="shared" si="27"/>
         <v>46053</v>
       </c>
-      <c r="R93" s="2">
-        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
-        <v>0</v>
-      </c>
-      <c r="S93">
+      <c r="R93" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>60</v>
+      </c>
+      <c r="S93" s="2">
+        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
         <v>0</v>
       </c>
       <c r="T93">
+        <v>0</v>
+      </c>
+      <c r="U93">
         <f t="shared" si="30"/>
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>44227</v>
       </c>
@@ -7086,19 +7466,23 @@
         <f t="shared" si="27"/>
         <v>44592</v>
       </c>
-      <c r="R94" s="2">
-        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
-        <v>0</v>
-      </c>
-      <c r="S94">
+      <c r="R94" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>12</v>
+      </c>
+      <c r="S94" s="2">
+        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
         <v>0</v>
       </c>
       <c r="T94">
+        <v>0</v>
+      </c>
+      <c r="U94">
         <f t="shared" si="30"/>
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>44227</v>
       </c>
@@ -7155,19 +7539,23 @@
         <f t="shared" si="27"/>
         <v>46053</v>
       </c>
-      <c r="R95" s="2">
-        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
-        <v>0</v>
-      </c>
-      <c r="S95">
+      <c r="R95" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>60</v>
+      </c>
+      <c r="S95" s="2">
+        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
         <v>0</v>
       </c>
       <c r="T95">
+        <v>0</v>
+      </c>
+      <c r="U95">
         <f t="shared" si="30"/>
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>44227</v>
       </c>
@@ -7224,19 +7612,23 @@
         <f t="shared" si="27"/>
         <v>46053</v>
       </c>
-      <c r="R96" s="2">
-        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
-        <v>0</v>
-      </c>
-      <c r="S96">
+      <c r="R96" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>60</v>
+      </c>
+      <c r="S96" s="2">
+        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
         <v>0</v>
       </c>
       <c r="T96">
+        <v>0</v>
+      </c>
+      <c r="U96">
         <f t="shared" si="30"/>
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>44227</v>
       </c>
@@ -7292,19 +7684,23 @@
         <f t="shared" si="27"/>
         <v>46053</v>
       </c>
-      <c r="R97" s="2">
+      <c r="R97" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>60</v>
+      </c>
+      <c r="S97" s="2">
         <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
         <v>142.85714285714286</v>
       </c>
-      <c r="S97">
-        <v>0</v>
-      </c>
       <c r="T97">
+        <v>0</v>
+      </c>
+      <c r="U97">
         <f t="shared" si="30"/>
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>44227</v>
       </c>
@@ -7360,19 +7756,23 @@
         <f t="shared" si="27"/>
         <v>46053</v>
       </c>
-      <c r="R98" s="2">
-        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
-        <v>100</v>
-      </c>
-      <c r="S98">
-        <v>0</v>
+      <c r="R98" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>60</v>
+      </c>
+      <c r="S98" s="2">
+        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
+        <v>100</v>
       </c>
       <c r="T98">
+        <v>0</v>
+      </c>
+      <c r="U98">
         <f t="shared" si="30"/>
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>44227</v>
       </c>
@@ -7428,19 +7828,23 @@
         <f t="shared" si="27"/>
         <v>46053</v>
       </c>
-      <c r="R99" s="2">
+      <c r="R99" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>60</v>
+      </c>
+      <c r="S99" s="2">
         <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
         <v>66.666666666666671</v>
       </c>
-      <c r="S99">
-        <v>0</v>
-      </c>
       <c r="T99">
+        <v>0</v>
+      </c>
+      <c r="U99">
         <f t="shared" si="30"/>
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>44227</v>
       </c>
@@ -7497,19 +7901,23 @@
         <f t="shared" si="27"/>
         <v>46053</v>
       </c>
-      <c r="R100" s="2">
-        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
-        <v>0</v>
-      </c>
-      <c r="S100">
+      <c r="R100" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>60</v>
+      </c>
+      <c r="S100" s="2">
+        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
+        <v>0</v>
+      </c>
+      <c r="T100">
         <v>1</v>
       </c>
-      <c r="T100">
+      <c r="U100">
         <f t="shared" si="30"/>
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>44227</v>
       </c>
@@ -7566,19 +7974,23 @@
         <f t="shared" si="27"/>
         <v>46053</v>
       </c>
-      <c r="R101" s="2">
-        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
-        <v>0</v>
-      </c>
-      <c r="S101">
+      <c r="R101" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>60</v>
+      </c>
+      <c r="S101" s="2">
+        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
+        <v>0</v>
+      </c>
+      <c r="T101">
         <v>2</v>
       </c>
-      <c r="T101">
+      <c r="U101">
         <f t="shared" si="30"/>
         <v>2</v>
       </c>
     </row>
-    <row r="102" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>44227</v>
       </c>
@@ -7635,19 +8047,23 @@
         <f t="shared" si="27"/>
         <v>46053</v>
       </c>
-      <c r="R102" s="2">
-        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
-        <v>0</v>
-      </c>
-      <c r="S102">
+      <c r="R102" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>60</v>
+      </c>
+      <c r="S102" s="2">
+        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
+        <v>0</v>
+      </c>
+      <c r="T102">
         <v>3</v>
       </c>
-      <c r="T102">
+      <c r="U102">
         <f t="shared" si="30"/>
         <v>3</v>
       </c>
     </row>
-    <row r="103" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>44227</v>
       </c>
@@ -7704,18 +8120,22 @@
         <f t="shared" si="27"/>
         <v>46053</v>
       </c>
-      <c r="R103" s="2">
-        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
-        <v>0</v>
-      </c>
-      <c r="S103">
+      <c r="R103" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>60</v>
+      </c>
+      <c r="S103" s="2">
+        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
         <v>0</v>
       </c>
       <c r="T103">
+        <v>0</v>
+      </c>
+      <c r="U103">
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>44227</v>
       </c>
@@ -7772,18 +8192,22 @@
         <f t="shared" si="27"/>
         <v>46053</v>
       </c>
-      <c r="R104" s="2">
-        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
-        <v>0</v>
-      </c>
-      <c r="S104">
+      <c r="R104" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>60</v>
+      </c>
+      <c r="S104" s="2">
+        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
         <v>0</v>
       </c>
       <c r="T104">
+        <v>0</v>
+      </c>
+      <c r="U104">
         <v>2</v>
       </c>
     </row>
-    <row r="105" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>44227</v>
       </c>
@@ -7840,18 +8264,22 @@
         <f t="shared" si="27"/>
         <v>46053</v>
       </c>
-      <c r="R105" s="2">
-        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
-        <v>0</v>
-      </c>
-      <c r="S105">
+      <c r="R105" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>60</v>
+      </c>
+      <c r="S105" s="2">
+        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
         <v>0</v>
       </c>
       <c r="T105">
+        <v>0</v>
+      </c>
+      <c r="U105">
         <v>3</v>
       </c>
     </row>
-    <row r="106" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>44227</v>
       </c>
@@ -7908,18 +8336,22 @@
         <f t="shared" si="27"/>
         <v>46053</v>
       </c>
-      <c r="R106" s="2">
-        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
-        <v>0</v>
-      </c>
-      <c r="S106">
+      <c r="R106" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>60</v>
+      </c>
+      <c r="S106" s="2">
+        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
         <v>0</v>
       </c>
       <c r="T106">
+        <v>0</v>
+      </c>
+      <c r="U106">
         <v>4</v>
       </c>
     </row>
-    <row r="107" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>44227</v>
       </c>
@@ -7976,19 +8408,23 @@
         <f t="shared" si="27"/>
         <v>46053</v>
       </c>
-      <c r="R107" s="2">
-        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
-        <v>0</v>
-      </c>
-      <c r="S107">
+      <c r="R107" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>60</v>
+      </c>
+      <c r="S107" s="2">
+        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
         <v>0</v>
       </c>
       <c r="T107">
-        <f t="shared" ref="T107:T117" si="31">S107</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="108" spans="1:20" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="U107">
+        <f t="shared" ref="U107:U117" si="31">T107</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>44227</v>
       </c>
@@ -8045,19 +8481,23 @@
         <f t="shared" si="27"/>
         <v>46053</v>
       </c>
-      <c r="R108" s="2">
-        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
-        <v>0</v>
-      </c>
-      <c r="S108">
+      <c r="R108" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>60</v>
+      </c>
+      <c r="S108" s="2">
+        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
         <v>0</v>
       </c>
       <c r="T108">
+        <v>0</v>
+      </c>
+      <c r="U108">
         <f t="shared" si="31"/>
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <v>44227</v>
       </c>
@@ -8114,19 +8554,23 @@
         <f t="shared" si="27"/>
         <v>44592</v>
       </c>
-      <c r="R109" s="2">
-        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
-        <v>0</v>
-      </c>
-      <c r="S109">
+      <c r="R109" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>12</v>
+      </c>
+      <c r="S109" s="2">
+        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
         <v>0</v>
       </c>
       <c r="T109">
+        <v>0</v>
+      </c>
+      <c r="U109">
         <f t="shared" si="31"/>
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
         <v>44227</v>
       </c>
@@ -8183,19 +8627,23 @@
         <f t="shared" si="27"/>
         <v>46053</v>
       </c>
-      <c r="R110" s="2">
-        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
-        <v>0</v>
-      </c>
-      <c r="S110">
+      <c r="R110" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>60</v>
+      </c>
+      <c r="S110" s="2">
+        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
         <v>0</v>
       </c>
       <c r="T110">
+        <v>0</v>
+      </c>
+      <c r="U110">
         <f t="shared" si="31"/>
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
         <v>44227</v>
       </c>
@@ -8252,19 +8700,23 @@
         <f t="shared" si="27"/>
         <v>46053</v>
       </c>
-      <c r="R111" s="2">
-        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
-        <v>0</v>
-      </c>
-      <c r="S111">
+      <c r="R111" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>60</v>
+      </c>
+      <c r="S111" s="2">
+        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
         <v>0</v>
       </c>
       <c r="T111">
+        <v>0</v>
+      </c>
+      <c r="U111">
         <f t="shared" si="31"/>
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
         <v>44227</v>
       </c>
@@ -8320,19 +8772,23 @@
         <f t="shared" si="27"/>
         <v>46053</v>
       </c>
-      <c r="R112" s="2">
+      <c r="R112" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>60</v>
+      </c>
+      <c r="S112" s="2">
         <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
         <v>142.85714285714286</v>
       </c>
-      <c r="S112">
-        <v>0</v>
-      </c>
       <c r="T112">
+        <v>0</v>
+      </c>
+      <c r="U112">
         <f t="shared" si="31"/>
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
         <v>44227</v>
       </c>
@@ -8388,19 +8844,23 @@
         <f t="shared" si="27"/>
         <v>46053</v>
       </c>
-      <c r="R113" s="2">
-        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
-        <v>100</v>
-      </c>
-      <c r="S113">
-        <v>0</v>
+      <c r="R113" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>60</v>
+      </c>
+      <c r="S113" s="2">
+        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
+        <v>100</v>
       </c>
       <c r="T113">
+        <v>0</v>
+      </c>
+      <c r="U113">
         <f t="shared" si="31"/>
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
         <v>44227</v>
       </c>
@@ -8456,19 +8916,23 @@
         <f t="shared" si="27"/>
         <v>46053</v>
       </c>
-      <c r="R114" s="2">
+      <c r="R114" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>60</v>
+      </c>
+      <c r="S114" s="2">
         <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
         <v>66.666666666666671</v>
       </c>
-      <c r="S114">
-        <v>0</v>
-      </c>
       <c r="T114">
+        <v>0</v>
+      </c>
+      <c r="U114">
         <f t="shared" si="31"/>
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
         <v>44227</v>
       </c>
@@ -8525,19 +8989,23 @@
         <f t="shared" si="27"/>
         <v>46053</v>
       </c>
-      <c r="R115" s="2">
-        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
-        <v>0</v>
-      </c>
-      <c r="S115">
+      <c r="R115" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>60</v>
+      </c>
+      <c r="S115" s="2">
+        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
+        <v>0</v>
+      </c>
+      <c r="T115">
         <v>1</v>
       </c>
-      <c r="T115">
+      <c r="U115">
         <f t="shared" si="31"/>
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
         <v>44227</v>
       </c>
@@ -8594,19 +9062,23 @@
         <f t="shared" si="27"/>
         <v>46053</v>
       </c>
-      <c r="R116" s="2">
-        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
-        <v>0</v>
-      </c>
-      <c r="S116">
+      <c r="R116" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>60</v>
+      </c>
+      <c r="S116" s="2">
+        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
+        <v>0</v>
+      </c>
+      <c r="T116">
         <v>2</v>
       </c>
-      <c r="T116">
+      <c r="U116">
         <f t="shared" si="31"/>
         <v>2</v>
       </c>
     </row>
-    <row r="117" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
         <v>44227</v>
       </c>
@@ -8663,19 +9135,23 @@
         <f t="shared" si="27"/>
         <v>46053</v>
       </c>
-      <c r="R117" s="2">
-        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
-        <v>0</v>
-      </c>
-      <c r="S117">
+      <c r="R117" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>60</v>
+      </c>
+      <c r="S117" s="2">
+        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
+        <v>0</v>
+      </c>
+      <c r="T117">
         <v>3</v>
       </c>
-      <c r="T117">
+      <c r="U117">
         <f t="shared" si="31"/>
         <v>3</v>
       </c>
     </row>
-    <row r="118" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
         <v>44227</v>
       </c>
@@ -8732,18 +9208,22 @@
         <f t="shared" si="27"/>
         <v>46053</v>
       </c>
-      <c r="R118" s="2">
-        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
-        <v>0</v>
-      </c>
-      <c r="S118">
+      <c r="R118" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>60</v>
+      </c>
+      <c r="S118" s="2">
+        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
         <v>0</v>
       </c>
       <c r="T118">
+        <v>0</v>
+      </c>
+      <c r="U118">
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
         <v>44227</v>
       </c>
@@ -8800,18 +9280,22 @@
         <f t="shared" si="27"/>
         <v>46053</v>
       </c>
-      <c r="R119" s="2">
-        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
-        <v>0</v>
-      </c>
-      <c r="S119">
+      <c r="R119" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>60</v>
+      </c>
+      <c r="S119" s="2">
+        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
         <v>0</v>
       </c>
       <c r="T119">
+        <v>0</v>
+      </c>
+      <c r="U119">
         <v>2</v>
       </c>
     </row>
-    <row r="120" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
         <v>44227</v>
       </c>
@@ -8868,18 +9352,22 @@
         <f t="shared" si="27"/>
         <v>46053</v>
       </c>
-      <c r="R120" s="2">
-        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
-        <v>0</v>
-      </c>
-      <c r="S120">
+      <c r="R120" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>60</v>
+      </c>
+      <c r="S120" s="2">
+        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
         <v>0</v>
       </c>
       <c r="T120">
+        <v>0</v>
+      </c>
+      <c r="U120">
         <v>3</v>
       </c>
     </row>
-    <row r="121" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
         <v>44227</v>
       </c>
@@ -8936,21 +9424,26 @@
         <f t="shared" ref="Q121" si="33">EOMONTH(D121,H121)</f>
         <v>46053</v>
       </c>
-      <c r="R121" s="2">
-        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
-        <v>0</v>
-      </c>
-      <c r="S121">
+      <c r="R121" s="4">
+        <f>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</f>
+        <v>60</v>
+      </c>
+      <c r="S121" s="2">
+        <f>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</f>
         <v>0</v>
       </c>
       <c r="T121">
+        <v>0</v>
+      </c>
+      <c r="U121">
         <v>4</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
us the transition matrix to calculate the probability of default and survival directly rather than from the calculating the cumulative and then marginal probabilities.
The full TM is now passed through the Z framework.

The probability of cure and write-off now need to be configured in the TTC TM. (see example)

Ratings now start at 1 rather than 0. The 0 rating is used for attrition.

The model can now cater for single and multiple default definitions via the TM approach.
</commit_message>
<xml_diff>
--- a/data/account_level_data.xlsx
+++ b/data/account_level_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\geyerbisschoff\PythonProjects\Z-model\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBD741DD-B6A5-4991-9E02-4DA774BDBA10}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49CD58D3-3329-4433-88CF-5AAB89E3F01C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1275" yWindow="-120" windowWidth="27645" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-40212" yWindow="-6528" windowWidth="40320" windowHeight="17496" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DATA" sheetId="1" r:id="rId1"/>
@@ -286,10 +286,10 @@
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
@@ -348,20 +348,18 @@
     <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="contractual_payment" dataDxfId="4">
       <calculatedColumnFormula>-PMT(M2/K2,DATEDIF(D2,Q2,"y")*I2,E2,-G2,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="maturity_date" dataDxfId="2">
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="maturity_date" dataDxfId="3">
       <calculatedColumnFormula>EOMONTH(D2,H2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="22" xr3:uid="{839146DB-6DF9-42EE-8D52-721111993876}" name="remaining_life" dataDxfId="0">
+    <tableColumn id="22" xr3:uid="{839146DB-6DF9-42EE-8D52-721111993876}" name="remaining_life" dataDxfId="2">
       <calculatedColumnFormula>DATEDIF(Table1[[#This Row],[reporting_date]],Table1[[#This Row],[maturity_date]],"m")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="collateral_value" dataDxfId="1">
       <calculatedColumnFormula>IF(ISNA(Table1[[#This Row],[ltv]]),0,Table1[[#This Row],[outstanding_balance]]/Table1[[#This Row],[ltv]])</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="origination_rating"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="current_rating">
-      <calculatedColumnFormula>T2</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="watchlist" dataDxfId="3"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="current_rating"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="watchlist" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -632,8 +630,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="R2" sqref="R2"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="X10" sqref="X10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -792,11 +790,10 @@
         <v>0</v>
       </c>
       <c r="T2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U2">
-        <f t="shared" ref="U2:U12" si="2">T2</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V2" s="4">
         <v>1</v>
@@ -852,11 +849,11 @@
         <v>0</v>
       </c>
       <c r="P3" s="2">
-        <f t="shared" ref="P3:P7" si="3">-PMT(M3/K3,DATEDIF(D3,Q3,"y")*I3,E3,-G3,0)</f>
+        <f t="shared" ref="P3:P7" si="2">-PMT(M3/K3,DATEDIF(D3,Q3,"y")*I3,E3,-G3,0)</f>
         <v>0.41666666666666669</v>
       </c>
       <c r="Q3" s="1">
-        <f t="shared" ref="Q3:Q7" si="4">EOMONTH(D3,H3)</f>
+        <f t="shared" ref="Q3:Q7" si="3">EOMONTH(D3,H3)</f>
         <v>45688</v>
       </c>
       <c r="R3" s="4">
@@ -868,11 +865,10 @@
         <v>0</v>
       </c>
       <c r="T3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U3">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V3" s="4">
         <v>2</v>
@@ -928,11 +924,11 @@
         <v>0</v>
       </c>
       <c r="P4" s="2">
+        <f t="shared" si="2"/>
+        <v>8.5607481788467137</v>
+      </c>
+      <c r="Q4" s="1">
         <f t="shared" si="3"/>
-        <v>8.5607481788467137</v>
-      </c>
-      <c r="Q4" s="1">
-        <f t="shared" si="4"/>
         <v>44227</v>
       </c>
       <c r="R4" s="4">
@@ -944,11 +940,10 @@
         <v>0</v>
       </c>
       <c r="T4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U4">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V4" s="4">
         <v>3</v>
@@ -1004,11 +999,11 @@
         <v>0</v>
       </c>
       <c r="P5" s="2">
+        <f t="shared" si="2"/>
+        <v>5.2216299555219434</v>
+      </c>
+      <c r="Q5" s="1">
         <f t="shared" si="3"/>
-        <v>5.2216299555219434</v>
-      </c>
-      <c r="Q5" s="1">
-        <f t="shared" si="4"/>
         <v>45688</v>
       </c>
       <c r="R5" s="4">
@@ -1020,11 +1015,10 @@
         <v>0</v>
       </c>
       <c r="T5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U5">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
@@ -1077,11 +1071,11 @@
         <v>0</v>
       </c>
       <c r="P6" s="2">
+        <f t="shared" si="2"/>
+        <v>1.8871233644010934</v>
+      </c>
+      <c r="Q6" s="1">
         <f t="shared" si="3"/>
-        <v>1.8871233644010934</v>
-      </c>
-      <c r="Q6" s="1">
-        <f t="shared" si="4"/>
         <v>45688</v>
       </c>
       <c r="R6" s="4">
@@ -1093,11 +1087,10 @@
         <v>0</v>
       </c>
       <c r="T6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U6">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
@@ -1149,11 +1142,11 @@
         <v>0</v>
       </c>
       <c r="P7" s="2">
+        <f t="shared" si="2"/>
+        <v>1.8871233644010934</v>
+      </c>
+      <c r="Q7" s="1">
         <f t="shared" si="3"/>
-        <v>1.8871233644010934</v>
-      </c>
-      <c r="Q7" s="1">
-        <f t="shared" si="4"/>
         <v>45688</v>
       </c>
       <c r="R7" s="4">
@@ -1165,11 +1158,10 @@
         <v>142.85714285714286</v>
       </c>
       <c r="T7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U7">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
@@ -1221,11 +1213,11 @@
         <v>0</v>
       </c>
       <c r="P8" s="2">
-        <f t="shared" ref="P8" si="5">-PMT(M8/K8,DATEDIF(D8,Q8,"y")*I8,E8,-G8,0)</f>
+        <f t="shared" ref="P8" si="4">-PMT(M8/K8,DATEDIF(D8,Q8,"y")*I8,E8,-G8,0)</f>
         <v>1.8871233644010934</v>
       </c>
       <c r="Q8" s="1">
-        <f t="shared" ref="Q8" si="6">EOMONTH(D8,H8)</f>
+        <f t="shared" ref="Q8" si="5">EOMONTH(D8,H8)</f>
         <v>45688</v>
       </c>
       <c r="R8" s="4">
@@ -1237,11 +1229,10 @@
         <v>100</v>
       </c>
       <c r="T8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U8">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
@@ -1293,11 +1284,11 @@
         <v>0</v>
       </c>
       <c r="P9" s="2">
-        <f t="shared" ref="P9:P10" si="7">-PMT(M9/K9,DATEDIF(D9,Q9,"y")*I9,E9,-G9,0)</f>
+        <f t="shared" ref="P9:P10" si="6">-PMT(M9/K9,DATEDIF(D9,Q9,"y")*I9,E9,-G9,0)</f>
         <v>1.8871233644010934</v>
       </c>
       <c r="Q9" s="1">
-        <f t="shared" ref="Q9:Q10" si="8">EOMONTH(D9,H9)</f>
+        <f t="shared" ref="Q9:Q10" si="7">EOMONTH(D9,H9)</f>
         <v>45688</v>
       </c>
       <c r="R9" s="4">
@@ -1309,11 +1300,10 @@
         <v>66.666666666666671</v>
       </c>
       <c r="T9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U9">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
@@ -1366,11 +1356,11 @@
         <v>0</v>
       </c>
       <c r="P10" s="2">
+        <f t="shared" si="6"/>
+        <v>1.8871233644010934</v>
+      </c>
+      <c r="Q10" s="1">
         <f t="shared" si="7"/>
-        <v>1.8871233644010934</v>
-      </c>
-      <c r="Q10" s="1">
-        <f t="shared" si="8"/>
         <v>45688</v>
       </c>
       <c r="R10" s="4">
@@ -1382,11 +1372,10 @@
         <v>0</v>
       </c>
       <c r="T10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U10">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
@@ -1439,11 +1428,11 @@
         <v>0</v>
       </c>
       <c r="P11" s="2">
-        <f t="shared" ref="P11" si="9">-PMT(M11/K11,DATEDIF(D11,Q11,"y")*I11,E11,-G11,0)</f>
+        <f t="shared" ref="P11" si="8">-PMT(M11/K11,DATEDIF(D11,Q11,"y")*I11,E11,-G11,0)</f>
         <v>1.8871233644010934</v>
       </c>
       <c r="Q11" s="1">
-        <f t="shared" ref="Q11" si="10">EOMONTH(D11,H11)</f>
+        <f t="shared" ref="Q11" si="9">EOMONTH(D11,H11)</f>
         <v>45688</v>
       </c>
       <c r="R11" s="4">
@@ -1455,11 +1444,10 @@
         <v>0</v>
       </c>
       <c r="T11">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="U11">
-        <f t="shared" si="2"/>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
@@ -1512,11 +1500,11 @@
         <v>0</v>
       </c>
       <c r="P12" s="2">
-        <f t="shared" ref="P12:P13" si="11">-PMT(M12/K12,DATEDIF(D12,Q12,"y")*I12,E12,-G12,0)</f>
+        <f t="shared" ref="P12:P13" si="10">-PMT(M12/K12,DATEDIF(D12,Q12,"y")*I12,E12,-G12,0)</f>
         <v>1.8871233644010934</v>
       </c>
       <c r="Q12" s="1">
-        <f t="shared" ref="Q12:Q13" si="12">EOMONTH(D12,H12)</f>
+        <f t="shared" ref="Q12:Q13" si="11">EOMONTH(D12,H12)</f>
         <v>45688</v>
       </c>
       <c r="R12" s="4">
@@ -1528,11 +1516,10 @@
         <v>0</v>
       </c>
       <c r="T12">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="U12">
-        <f t="shared" si="2"/>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
@@ -1585,11 +1572,11 @@
         <v>2</v>
       </c>
       <c r="P13" s="2">
+        <f t="shared" si="10"/>
+        <v>1.8871233644010934</v>
+      </c>
+      <c r="Q13" s="1">
         <f t="shared" si="11"/>
-        <v>1.8871233644010934</v>
-      </c>
-      <c r="Q13" s="1">
-        <f t="shared" si="12"/>
         <v>45688</v>
       </c>
       <c r="R13" s="4">
@@ -1601,10 +1588,10 @@
         <v>0</v>
       </c>
       <c r="T13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U13">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
@@ -1657,11 +1644,11 @@
         <v>2</v>
       </c>
       <c r="P14" s="2">
-        <f t="shared" ref="P14" si="13">-PMT(M14/K14,DATEDIF(D14,Q14,"y")*I14,E14,-G14,0)</f>
+        <f t="shared" ref="P14" si="12">-PMT(M14/K14,DATEDIF(D14,Q14,"y")*I14,E14,-G14,0)</f>
         <v>1.8871233644010934</v>
       </c>
       <c r="Q14" s="1">
-        <f t="shared" ref="Q14" si="14">EOMONTH(D14,H14)</f>
+        <f t="shared" ref="Q14" si="13">EOMONTH(D14,H14)</f>
         <v>45688</v>
       </c>
       <c r="R14" s="4">
@@ -1673,10 +1660,10 @@
         <v>0</v>
       </c>
       <c r="T14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U14">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
@@ -1729,11 +1716,11 @@
         <v>2</v>
       </c>
       <c r="P15" s="2">
-        <f t="shared" ref="P15" si="15">-PMT(M15/K15,DATEDIF(D15,Q15,"y")*I15,E15,-G15,0)</f>
+        <f t="shared" ref="P15" si="14">-PMT(M15/K15,DATEDIF(D15,Q15,"y")*I15,E15,-G15,0)</f>
         <v>1.8871233644010934</v>
       </c>
       <c r="Q15" s="1">
-        <f t="shared" ref="Q15" si="16">EOMONTH(D15,H15)</f>
+        <f t="shared" ref="Q15" si="15">EOMONTH(D15,H15)</f>
         <v>45688</v>
       </c>
       <c r="R15" s="4">
@@ -1745,10 +1732,10 @@
         <v>0</v>
       </c>
       <c r="T15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U15">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
@@ -1801,11 +1788,11 @@
         <v>2</v>
       </c>
       <c r="P16" s="2">
-        <f t="shared" ref="P16:P30" si="17">-PMT(M16/K16,DATEDIF(D16,Q16,"y")*I16,E16,-G16,0)</f>
+        <f t="shared" ref="P16:P30" si="16">-PMT(M16/K16,DATEDIF(D16,Q16,"y")*I16,E16,-G16,0)</f>
         <v>1.8871233644010934</v>
       </c>
       <c r="Q16" s="1">
-        <f t="shared" ref="Q16:Q30" si="18">EOMONTH(D16,H16)</f>
+        <f t="shared" ref="Q16:Q30" si="17">EOMONTH(D16,H16)</f>
         <v>45688</v>
       </c>
       <c r="R16" s="4">
@@ -1817,10 +1804,10 @@
         <v>0</v>
       </c>
       <c r="T16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U16">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
@@ -1873,11 +1860,11 @@
         <v>0</v>
       </c>
       <c r="P17" s="2">
+        <f t="shared" si="16"/>
+        <v>1.8871233644010934</v>
+      </c>
+      <c r="Q17" s="1">
         <f t="shared" si="17"/>
-        <v>1.8871233644010934</v>
-      </c>
-      <c r="Q17" s="1">
-        <f t="shared" si="18"/>
         <v>45688</v>
       </c>
       <c r="R17" s="4">
@@ -1889,11 +1876,10 @@
         <v>0</v>
       </c>
       <c r="T17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U17">
-        <f t="shared" ref="U17:U27" si="19">T17</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
@@ -1946,11 +1932,11 @@
         <v>0</v>
       </c>
       <c r="P18" s="2">
+        <f t="shared" si="16"/>
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="Q18" s="1">
         <f t="shared" si="17"/>
-        <v>0.41666666666666669</v>
-      </c>
-      <c r="Q18" s="1">
-        <f t="shared" si="18"/>
         <v>45688</v>
       </c>
       <c r="R18" s="4">
@@ -1962,11 +1948,10 @@
         <v>0</v>
       </c>
       <c r="T18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U18">
-        <f t="shared" si="19"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
@@ -2019,11 +2004,11 @@
         <v>0</v>
       </c>
       <c r="P19" s="2">
+        <f t="shared" si="16"/>
+        <v>8.5607481788467137</v>
+      </c>
+      <c r="Q19" s="1">
         <f t="shared" si="17"/>
-        <v>8.5607481788467137</v>
-      </c>
-      <c r="Q19" s="1">
-        <f t="shared" si="18"/>
         <v>44227</v>
       </c>
       <c r="R19" s="4">
@@ -2035,11 +2020,10 @@
         <v>0</v>
       </c>
       <c r="T19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U19">
-        <f t="shared" si="19"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
@@ -2092,11 +2076,11 @@
         <v>0</v>
       </c>
       <c r="P20" s="2">
+        <f t="shared" si="16"/>
+        <v>5.2216299555219434</v>
+      </c>
+      <c r="Q20" s="1">
         <f t="shared" si="17"/>
-        <v>5.2216299555219434</v>
-      </c>
-      <c r="Q20" s="1">
-        <f t="shared" si="18"/>
         <v>45688</v>
       </c>
       <c r="R20" s="4">
@@ -2108,11 +2092,10 @@
         <v>0</v>
       </c>
       <c r="T20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U20">
-        <f t="shared" si="19"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
@@ -2165,11 +2148,11 @@
         <v>0</v>
       </c>
       <c r="P21" s="2">
+        <f t="shared" si="16"/>
+        <v>1.8871233644010934</v>
+      </c>
+      <c r="Q21" s="1">
         <f t="shared" si="17"/>
-        <v>1.8871233644010934</v>
-      </c>
-      <c r="Q21" s="1">
-        <f t="shared" si="18"/>
         <v>45688</v>
       </c>
       <c r="R21" s="4">
@@ -2181,11 +2164,10 @@
         <v>0</v>
       </c>
       <c r="T21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U21">
-        <f t="shared" si="19"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.25">
@@ -2237,11 +2219,11 @@
         <v>0</v>
       </c>
       <c r="P22" s="2">
+        <f t="shared" si="16"/>
+        <v>1.8871233644010934</v>
+      </c>
+      <c r="Q22" s="1">
         <f t="shared" si="17"/>
-        <v>1.8871233644010934</v>
-      </c>
-      <c r="Q22" s="1">
-        <f t="shared" si="18"/>
         <v>45688</v>
       </c>
       <c r="R22" s="4">
@@ -2253,11 +2235,10 @@
         <v>142.85714285714286</v>
       </c>
       <c r="T22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U22">
-        <f t="shared" si="19"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.25">
@@ -2309,11 +2290,11 @@
         <v>0</v>
       </c>
       <c r="P23" s="2">
+        <f t="shared" si="16"/>
+        <v>1.8871233644010934</v>
+      </c>
+      <c r="Q23" s="1">
         <f t="shared" si="17"/>
-        <v>1.8871233644010934</v>
-      </c>
-      <c r="Q23" s="1">
-        <f t="shared" si="18"/>
         <v>45688</v>
       </c>
       <c r="R23" s="4">
@@ -2325,11 +2306,10 @@
         <v>100</v>
       </c>
       <c r="T23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U23">
-        <f t="shared" si="19"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.25">
@@ -2381,11 +2361,11 @@
         <v>0</v>
       </c>
       <c r="P24" s="2">
+        <f t="shared" si="16"/>
+        <v>1.8871233644010934</v>
+      </c>
+      <c r="Q24" s="1">
         <f t="shared" si="17"/>
-        <v>1.8871233644010934</v>
-      </c>
-      <c r="Q24" s="1">
-        <f t="shared" si="18"/>
         <v>45688</v>
       </c>
       <c r="R24" s="4">
@@ -2397,11 +2377,10 @@
         <v>66.666666666666671</v>
       </c>
       <c r="T24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U24">
-        <f t="shared" si="19"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.25">
@@ -2454,11 +2433,11 @@
         <v>0</v>
       </c>
       <c r="P25" s="2">
+        <f t="shared" si="16"/>
+        <v>1.8871233644010934</v>
+      </c>
+      <c r="Q25" s="1">
         <f t="shared" si="17"/>
-        <v>1.8871233644010934</v>
-      </c>
-      <c r="Q25" s="1">
-        <f t="shared" si="18"/>
         <v>45688</v>
       </c>
       <c r="R25" s="4">
@@ -2470,11 +2449,10 @@
         <v>0</v>
       </c>
       <c r="T25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U25">
-        <f t="shared" si="19"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.25">
@@ -2527,11 +2505,11 @@
         <v>0</v>
       </c>
       <c r="P26" s="2">
+        <f t="shared" si="16"/>
+        <v>1.8871233644010934</v>
+      </c>
+      <c r="Q26" s="1">
         <f t="shared" si="17"/>
-        <v>1.8871233644010934</v>
-      </c>
-      <c r="Q26" s="1">
-        <f t="shared" si="18"/>
         <v>45688</v>
       </c>
       <c r="R26" s="4">
@@ -2543,11 +2521,10 @@
         <v>0</v>
       </c>
       <c r="T26">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="U26">
-        <f t="shared" si="19"/>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.25">
@@ -2600,11 +2577,11 @@
         <v>0</v>
       </c>
       <c r="P27" s="2">
+        <f t="shared" si="16"/>
+        <v>1.8871233644010934</v>
+      </c>
+      <c r="Q27" s="1">
         <f t="shared" si="17"/>
-        <v>1.8871233644010934</v>
-      </c>
-      <c r="Q27" s="1">
-        <f t="shared" si="18"/>
         <v>45688</v>
       </c>
       <c r="R27" s="4">
@@ -2616,11 +2593,10 @@
         <v>0</v>
       </c>
       <c r="T27">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="U27">
-        <f t="shared" si="19"/>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.25">
@@ -2673,11 +2649,11 @@
         <v>2</v>
       </c>
       <c r="P28" s="2">
+        <f t="shared" si="16"/>
+        <v>1.8871233644010934</v>
+      </c>
+      <c r="Q28" s="1">
         <f t="shared" si="17"/>
-        <v>1.8871233644010934</v>
-      </c>
-      <c r="Q28" s="1">
-        <f t="shared" si="18"/>
         <v>45688</v>
       </c>
       <c r="R28" s="4">
@@ -2689,10 +2665,10 @@
         <v>0</v>
       </c>
       <c r="T28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U28">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.25">
@@ -2745,11 +2721,11 @@
         <v>2</v>
       </c>
       <c r="P29" s="2">
+        <f t="shared" si="16"/>
+        <v>1.8871233644010934</v>
+      </c>
+      <c r="Q29" s="1">
         <f t="shared" si="17"/>
-        <v>1.8871233644010934</v>
-      </c>
-      <c r="Q29" s="1">
-        <f t="shared" si="18"/>
         <v>45688</v>
       </c>
       <c r="R29" s="4">
@@ -2761,10 +2737,10 @@
         <v>0</v>
       </c>
       <c r="T29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U29">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.25">
@@ -2817,11 +2793,11 @@
         <v>2</v>
       </c>
       <c r="P30" s="2">
+        <f t="shared" si="16"/>
+        <v>1.8871233644010934</v>
+      </c>
+      <c r="Q30" s="1">
         <f t="shared" si="17"/>
-        <v>1.8871233644010934</v>
-      </c>
-      <c r="Q30" s="1">
-        <f t="shared" si="18"/>
         <v>45688</v>
       </c>
       <c r="R30" s="4">
@@ -2833,10 +2809,10 @@
         <v>0</v>
       </c>
       <c r="T30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U30">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.25">
@@ -2889,11 +2865,11 @@
         <v>2</v>
       </c>
       <c r="P31" s="2">
-        <f t="shared" ref="P31:P45" si="20">-PMT(M31/K31,DATEDIF(D31,Q31,"y")*I31,E31,-G31,0)</f>
+        <f t="shared" ref="P31:P45" si="18">-PMT(M31/K31,DATEDIF(D31,Q31,"y")*I31,E31,-G31,0)</f>
         <v>1.8871233644010934</v>
       </c>
       <c r="Q31" s="1">
-        <f t="shared" ref="Q31:Q45" si="21">EOMONTH(D31,H31)</f>
+        <f t="shared" ref="Q31:Q45" si="19">EOMONTH(D31,H31)</f>
         <v>45688</v>
       </c>
       <c r="R31" s="4">
@@ -2905,10 +2881,10 @@
         <v>0</v>
       </c>
       <c r="T31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U31">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.25">
@@ -2961,11 +2937,11 @@
         <v>0</v>
       </c>
       <c r="P32" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="18"/>
         <v>1.8871233644010934</v>
       </c>
       <c r="Q32" s="1">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>45688</v>
       </c>
       <c r="R32" s="4">
@@ -2977,11 +2953,10 @@
         <v>0</v>
       </c>
       <c r="T32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U32">
-        <f t="shared" ref="U32:U42" si="22">T32</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.25">
@@ -3034,11 +3009,11 @@
         <v>0</v>
       </c>
       <c r="P33" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="18"/>
         <v>0.41666666666666669</v>
       </c>
       <c r="Q33" s="1">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>45688</v>
       </c>
       <c r="R33" s="4">
@@ -3050,11 +3025,10 @@
         <v>0</v>
       </c>
       <c r="T33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U33">
-        <f t="shared" si="22"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.25">
@@ -3107,11 +3081,11 @@
         <v>0</v>
       </c>
       <c r="P34" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="18"/>
         <v>8.5607481788467137</v>
       </c>
       <c r="Q34" s="1">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>44227</v>
       </c>
       <c r="R34" s="4">
@@ -3123,11 +3097,10 @@
         <v>0</v>
       </c>
       <c r="T34">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U34">
-        <f t="shared" si="22"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:21" x14ac:dyDescent="0.25">
@@ -3180,11 +3153,11 @@
         <v>0</v>
       </c>
       <c r="P35" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="18"/>
         <v>5.2216299555219434</v>
       </c>
       <c r="Q35" s="1">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>45688</v>
       </c>
       <c r="R35" s="4">
@@ -3196,11 +3169,10 @@
         <v>0</v>
       </c>
       <c r="T35">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U35">
-        <f t="shared" si="22"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.25">
@@ -3253,11 +3225,11 @@
         <v>0</v>
       </c>
       <c r="P36" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="18"/>
         <v>1.8871233644010934</v>
       </c>
       <c r="Q36" s="1">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>45688</v>
       </c>
       <c r="R36" s="4">
@@ -3269,11 +3241,10 @@
         <v>0</v>
       </c>
       <c r="T36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U36">
-        <f t="shared" si="22"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.25">
@@ -3325,11 +3296,11 @@
         <v>0</v>
       </c>
       <c r="P37" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="18"/>
         <v>1.8871233644010934</v>
       </c>
       <c r="Q37" s="1">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>45688</v>
       </c>
       <c r="R37" s="4">
@@ -3341,11 +3312,10 @@
         <v>142.85714285714286</v>
       </c>
       <c r="T37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U37">
-        <f t="shared" si="22"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.25">
@@ -3397,11 +3367,11 @@
         <v>0</v>
       </c>
       <c r="P38" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="18"/>
         <v>1.8871233644010934</v>
       </c>
       <c r="Q38" s="1">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>45688</v>
       </c>
       <c r="R38" s="4">
@@ -3413,11 +3383,10 @@
         <v>100</v>
       </c>
       <c r="T38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U38">
-        <f t="shared" si="22"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.25">
@@ -3469,11 +3438,11 @@
         <v>0</v>
       </c>
       <c r="P39" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="18"/>
         <v>1.8871233644010934</v>
       </c>
       <c r="Q39" s="1">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>45688</v>
       </c>
       <c r="R39" s="4">
@@ -3485,11 +3454,10 @@
         <v>66.666666666666671</v>
       </c>
       <c r="T39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U39">
-        <f t="shared" si="22"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.25">
@@ -3542,11 +3510,11 @@
         <v>0</v>
       </c>
       <c r="P40" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="18"/>
         <v>1.8871233644010934</v>
       </c>
       <c r="Q40" s="1">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>45688</v>
       </c>
       <c r="R40" s="4">
@@ -3558,11 +3526,10 @@
         <v>0</v>
       </c>
       <c r="T40">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U40">
-        <f t="shared" si="22"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="41" spans="1:21" x14ac:dyDescent="0.25">
@@ -3615,11 +3582,11 @@
         <v>0</v>
       </c>
       <c r="P41" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="18"/>
         <v>1.8871233644010934</v>
       </c>
       <c r="Q41" s="1">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>45688</v>
       </c>
       <c r="R41" s="4">
@@ -3631,11 +3598,10 @@
         <v>0</v>
       </c>
       <c r="T41">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="U41">
-        <f t="shared" si="22"/>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.25">
@@ -3688,11 +3654,11 @@
         <v>0</v>
       </c>
       <c r="P42" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="18"/>
         <v>1.8871233644010934</v>
       </c>
       <c r="Q42" s="1">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>45688</v>
       </c>
       <c r="R42" s="4">
@@ -3704,11 +3670,10 @@
         <v>0</v>
       </c>
       <c r="T42">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="U42">
-        <f t="shared" si="22"/>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.25">
@@ -3761,11 +3726,11 @@
         <v>2</v>
       </c>
       <c r="P43" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="18"/>
         <v>1.8871233644010934</v>
       </c>
       <c r="Q43" s="1">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>45688</v>
       </c>
       <c r="R43" s="4">
@@ -3777,10 +3742,10 @@
         <v>0</v>
       </c>
       <c r="T43">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U43">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="44" spans="1:21" x14ac:dyDescent="0.25">
@@ -3833,11 +3798,11 @@
         <v>2</v>
       </c>
       <c r="P44" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="18"/>
         <v>1.8871233644010934</v>
       </c>
       <c r="Q44" s="1">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>45688</v>
       </c>
       <c r="R44" s="4">
@@ -3849,10 +3814,10 @@
         <v>0</v>
       </c>
       <c r="T44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U44">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="45" spans="1:21" x14ac:dyDescent="0.25">
@@ -3905,11 +3870,11 @@
         <v>2</v>
       </c>
       <c r="P45" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="18"/>
         <v>1.8871233644010934</v>
       </c>
       <c r="Q45" s="1">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>45688</v>
       </c>
       <c r="R45" s="4">
@@ -3921,10 +3886,10 @@
         <v>0</v>
       </c>
       <c r="T45">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U45">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="46" spans="1:21" x14ac:dyDescent="0.25">
@@ -3977,11 +3942,11 @@
         <v>2</v>
       </c>
       <c r="P46" s="2">
-        <f t="shared" ref="P46:P60" si="23">-PMT(M46/K46,DATEDIF(D46,Q46,"y")*I46,E46,-G46,0)</f>
+        <f t="shared" ref="P46:P60" si="20">-PMT(M46/K46,DATEDIF(D46,Q46,"y")*I46,E46,-G46,0)</f>
         <v>1.8871233644010934</v>
       </c>
       <c r="Q46" s="1">
-        <f t="shared" ref="Q46:Q60" si="24">EOMONTH(D46,H46)</f>
+        <f t="shared" ref="Q46:Q60" si="21">EOMONTH(D46,H46)</f>
         <v>45688</v>
       </c>
       <c r="R46" s="4">
@@ -3993,10 +3958,10 @@
         <v>0</v>
       </c>
       <c r="T46">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U46">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="47" spans="1:21" x14ac:dyDescent="0.25">
@@ -4049,11 +4014,11 @@
         <v>0</v>
       </c>
       <c r="P47" s="2">
-        <f t="shared" si="23"/>
+        <f t="shared" si="20"/>
         <v>1.8871233644010934</v>
       </c>
       <c r="Q47" s="1">
-        <f t="shared" si="24"/>
+        <f t="shared" si="21"/>
         <v>45688</v>
       </c>
       <c r="R47" s="4">
@@ -4065,11 +4030,10 @@
         <v>0</v>
       </c>
       <c r="T47">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U47">
-        <f t="shared" ref="U47:U57" si="25">T47</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:21" x14ac:dyDescent="0.25">
@@ -4122,11 +4086,11 @@
         <v>0</v>
       </c>
       <c r="P48" s="2">
-        <f t="shared" si="23"/>
+        <f t="shared" si="20"/>
         <v>0.41666666666666669</v>
       </c>
       <c r="Q48" s="1">
-        <f t="shared" si="24"/>
+        <f t="shared" si="21"/>
         <v>45688</v>
       </c>
       <c r="R48" s="4">
@@ -4138,11 +4102,10 @@
         <v>0</v>
       </c>
       <c r="T48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U48">
-        <f t="shared" si="25"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:21" x14ac:dyDescent="0.25">
@@ -4195,11 +4158,11 @@
         <v>0</v>
       </c>
       <c r="P49" s="2">
-        <f t="shared" si="23"/>
+        <f t="shared" si="20"/>
         <v>8.5607481788467137</v>
       </c>
       <c r="Q49" s="1">
-        <f t="shared" si="24"/>
+        <f t="shared" si="21"/>
         <v>44227</v>
       </c>
       <c r="R49" s="4">
@@ -4211,11 +4174,10 @@
         <v>0</v>
       </c>
       <c r="T49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U49">
-        <f t="shared" si="25"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:21" x14ac:dyDescent="0.25">
@@ -4268,11 +4230,11 @@
         <v>0</v>
       </c>
       <c r="P50" s="2">
-        <f t="shared" si="23"/>
+        <f t="shared" si="20"/>
         <v>5.2216299555219434</v>
       </c>
       <c r="Q50" s="1">
-        <f t="shared" si="24"/>
+        <f t="shared" si="21"/>
         <v>45688</v>
       </c>
       <c r="R50" s="4">
@@ -4284,11 +4246,10 @@
         <v>0</v>
       </c>
       <c r="T50">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U50">
-        <f t="shared" si="25"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:21" x14ac:dyDescent="0.25">
@@ -4341,11 +4302,11 @@
         <v>0</v>
       </c>
       <c r="P51" s="2">
-        <f t="shared" si="23"/>
+        <f t="shared" si="20"/>
         <v>1.8871233644010934</v>
       </c>
       <c r="Q51" s="1">
-        <f t="shared" si="24"/>
+        <f t="shared" si="21"/>
         <v>45688</v>
       </c>
       <c r="R51" s="4">
@@ -4357,11 +4318,10 @@
         <v>0</v>
       </c>
       <c r="T51">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U51">
-        <f t="shared" si="25"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:21" x14ac:dyDescent="0.25">
@@ -4413,11 +4373,11 @@
         <v>0</v>
       </c>
       <c r="P52" s="2">
-        <f t="shared" si="23"/>
+        <f t="shared" si="20"/>
         <v>1.8871233644010934</v>
       </c>
       <c r="Q52" s="1">
-        <f t="shared" si="24"/>
+        <f t="shared" si="21"/>
         <v>45688</v>
       </c>
       <c r="R52" s="4">
@@ -4429,11 +4389,10 @@
         <v>142.85714285714286</v>
       </c>
       <c r="T52">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U52">
-        <f t="shared" si="25"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="53" spans="1:21" x14ac:dyDescent="0.25">
@@ -4485,11 +4444,11 @@
         <v>0</v>
       </c>
       <c r="P53" s="2">
-        <f t="shared" si="23"/>
+        <f t="shared" si="20"/>
         <v>1.8871233644010934</v>
       </c>
       <c r="Q53" s="1">
-        <f t="shared" si="24"/>
+        <f t="shared" si="21"/>
         <v>45688</v>
       </c>
       <c r="R53" s="4">
@@ -4501,11 +4460,10 @@
         <v>100</v>
       </c>
       <c r="T53">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U53">
-        <f t="shared" si="25"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:21" x14ac:dyDescent="0.25">
@@ -4557,11 +4515,11 @@
         <v>0</v>
       </c>
       <c r="P54" s="2">
-        <f t="shared" si="23"/>
+        <f t="shared" si="20"/>
         <v>1.8871233644010934</v>
       </c>
       <c r="Q54" s="1">
-        <f t="shared" si="24"/>
+        <f t="shared" si="21"/>
         <v>45688</v>
       </c>
       <c r="R54" s="4">
@@ -4573,11 +4531,10 @@
         <v>66.666666666666671</v>
       </c>
       <c r="T54">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U54">
-        <f t="shared" si="25"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:21" x14ac:dyDescent="0.25">
@@ -4630,11 +4587,11 @@
         <v>0</v>
       </c>
       <c r="P55" s="2">
-        <f t="shared" si="23"/>
+        <f t="shared" si="20"/>
         <v>1.8871233644010934</v>
       </c>
       <c r="Q55" s="1">
-        <f t="shared" si="24"/>
+        <f t="shared" si="21"/>
         <v>45688</v>
       </c>
       <c r="R55" s="4">
@@ -4646,11 +4603,10 @@
         <v>0</v>
       </c>
       <c r="T55">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U55">
-        <f t="shared" si="25"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="56" spans="1:21" x14ac:dyDescent="0.25">
@@ -4703,11 +4659,11 @@
         <v>0</v>
       </c>
       <c r="P56" s="2">
-        <f t="shared" si="23"/>
+        <f t="shared" si="20"/>
         <v>1.8871233644010934</v>
       </c>
       <c r="Q56" s="1">
-        <f t="shared" si="24"/>
+        <f t="shared" si="21"/>
         <v>45688</v>
       </c>
       <c r="R56" s="4">
@@ -4719,11 +4675,10 @@
         <v>0</v>
       </c>
       <c r="T56">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="U56">
-        <f t="shared" si="25"/>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="57" spans="1:21" x14ac:dyDescent="0.25">
@@ -4776,11 +4731,11 @@
         <v>0</v>
       </c>
       <c r="P57" s="2">
-        <f t="shared" si="23"/>
+        <f t="shared" si="20"/>
         <v>1.8871233644010934</v>
       </c>
       <c r="Q57" s="1">
-        <f t="shared" si="24"/>
+        <f t="shared" si="21"/>
         <v>45688</v>
       </c>
       <c r="R57" s="4">
@@ -4792,11 +4747,10 @@
         <v>0</v>
       </c>
       <c r="T57">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="U57">
-        <f t="shared" si="25"/>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="58" spans="1:21" x14ac:dyDescent="0.25">
@@ -4849,11 +4803,11 @@
         <v>2</v>
       </c>
       <c r="P58" s="2">
-        <f t="shared" si="23"/>
+        <f t="shared" si="20"/>
         <v>1.8871233644010934</v>
       </c>
       <c r="Q58" s="1">
-        <f t="shared" si="24"/>
+        <f t="shared" si="21"/>
         <v>45688</v>
       </c>
       <c r="R58" s="4">
@@ -4865,10 +4819,10 @@
         <v>0</v>
       </c>
       <c r="T58">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U58">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="59" spans="1:21" x14ac:dyDescent="0.25">
@@ -4921,11 +4875,11 @@
         <v>2</v>
       </c>
       <c r="P59" s="2">
-        <f t="shared" si="23"/>
+        <f t="shared" si="20"/>
         <v>1.8871233644010934</v>
       </c>
       <c r="Q59" s="1">
-        <f t="shared" si="24"/>
+        <f t="shared" si="21"/>
         <v>45688</v>
       </c>
       <c r="R59" s="4">
@@ -4937,10 +4891,10 @@
         <v>0</v>
       </c>
       <c r="T59">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U59">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="60" spans="1:21" x14ac:dyDescent="0.25">
@@ -4993,11 +4947,11 @@
         <v>2</v>
       </c>
       <c r="P60" s="2">
-        <f t="shared" si="23"/>
+        <f t="shared" si="20"/>
         <v>1.8871233644010934</v>
       </c>
       <c r="Q60" s="1">
-        <f t="shared" si="24"/>
+        <f t="shared" si="21"/>
         <v>45688</v>
       </c>
       <c r="R60" s="4">
@@ -5009,10 +4963,10 @@
         <v>0</v>
       </c>
       <c r="T60">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U60">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="61" spans="1:21" x14ac:dyDescent="0.25">
@@ -5065,11 +5019,11 @@
         <v>2</v>
       </c>
       <c r="P61" s="2">
-        <f t="shared" ref="P61:P120" si="26">-PMT(M61/K61,DATEDIF(D61,Q61,"y")*I61,E61,-G61,0)</f>
+        <f t="shared" ref="P61:P120" si="22">-PMT(M61/K61,DATEDIF(D61,Q61,"y")*I61,E61,-G61,0)</f>
         <v>1.8871233644010934</v>
       </c>
       <c r="Q61" s="1">
-        <f t="shared" ref="Q61:Q120" si="27">EOMONTH(D61,H61)</f>
+        <f t="shared" ref="Q61:Q120" si="23">EOMONTH(D61,H61)</f>
         <v>45688</v>
       </c>
       <c r="R61" s="4">
@@ -5081,10 +5035,10 @@
         <v>0</v>
       </c>
       <c r="T61">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U61">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="62" spans="1:21" x14ac:dyDescent="0.25">
@@ -5137,11 +5091,11 @@
         <v>0</v>
       </c>
       <c r="P62" s="2">
-        <f t="shared" si="26"/>
+        <f t="shared" si="22"/>
         <v>1.8871233644010934</v>
       </c>
       <c r="Q62" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="23"/>
         <v>46053</v>
       </c>
       <c r="R62" s="4">
@@ -5153,11 +5107,10 @@
         <v>0</v>
       </c>
       <c r="T62">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U62">
-        <f t="shared" ref="U62:U72" si="28">T62</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="63" spans="1:21" x14ac:dyDescent="0.25">
@@ -5210,11 +5163,11 @@
         <v>0</v>
       </c>
       <c r="P63" s="2">
-        <f t="shared" si="26"/>
+        <f t="shared" si="22"/>
         <v>0.41666666666666669</v>
       </c>
       <c r="Q63" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="23"/>
         <v>46053</v>
       </c>
       <c r="R63" s="4">
@@ -5226,11 +5179,10 @@
         <v>0</v>
       </c>
       <c r="T63">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U63">
-        <f t="shared" si="28"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="64" spans="1:21" x14ac:dyDescent="0.25">
@@ -5283,11 +5235,11 @@
         <v>0</v>
       </c>
       <c r="P64" s="2">
-        <f t="shared" si="26"/>
+        <f t="shared" si="22"/>
         <v>8.5607481788467137</v>
       </c>
       <c r="Q64" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="23"/>
         <v>44592</v>
       </c>
       <c r="R64" s="4">
@@ -5299,11 +5251,10 @@
         <v>0</v>
       </c>
       <c r="T64">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U64">
-        <f t="shared" si="28"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="65" spans="1:21" x14ac:dyDescent="0.25">
@@ -5356,11 +5307,11 @@
         <v>0</v>
       </c>
       <c r="P65" s="2">
-        <f t="shared" si="26"/>
+        <f t="shared" si="22"/>
         <v>5.2216299555219434</v>
       </c>
       <c r="Q65" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="23"/>
         <v>46053</v>
       </c>
       <c r="R65" s="4">
@@ -5372,11 +5323,10 @@
         <v>0</v>
       </c>
       <c r="T65">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U65">
-        <f t="shared" si="28"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="66" spans="1:21" x14ac:dyDescent="0.25">
@@ -5429,11 +5379,11 @@
         <v>0</v>
       </c>
       <c r="P66" s="2">
-        <f t="shared" si="26"/>
+        <f t="shared" si="22"/>
         <v>1.8871233644010934</v>
       </c>
       <c r="Q66" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="23"/>
         <v>46053</v>
       </c>
       <c r="R66" s="4">
@@ -5445,11 +5395,10 @@
         <v>0</v>
       </c>
       <c r="T66">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U66">
-        <f t="shared" si="28"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="67" spans="1:21" x14ac:dyDescent="0.25">
@@ -5501,11 +5450,11 @@
         <v>0</v>
       </c>
       <c r="P67" s="2">
-        <f t="shared" si="26"/>
+        <f t="shared" si="22"/>
         <v>1.8871233644010934</v>
       </c>
       <c r="Q67" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="23"/>
         <v>46053</v>
       </c>
       <c r="R67" s="4">
@@ -5517,11 +5466,10 @@
         <v>142.85714285714286</v>
       </c>
       <c r="T67">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U67">
-        <f t="shared" si="28"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="68" spans="1:21" x14ac:dyDescent="0.25">
@@ -5573,11 +5521,11 @@
         <v>0</v>
       </c>
       <c r="P68" s="2">
-        <f t="shared" si="26"/>
+        <f t="shared" si="22"/>
         <v>1.8871233644010934</v>
       </c>
       <c r="Q68" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="23"/>
         <v>46053</v>
       </c>
       <c r="R68" s="4">
@@ -5589,11 +5537,10 @@
         <v>100</v>
       </c>
       <c r="T68">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U68">
-        <f t="shared" si="28"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="69" spans="1:21" x14ac:dyDescent="0.25">
@@ -5645,11 +5592,11 @@
         <v>0</v>
       </c>
       <c r="P69" s="2">
-        <f t="shared" si="26"/>
+        <f t="shared" si="22"/>
         <v>1.8871233644010934</v>
       </c>
       <c r="Q69" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="23"/>
         <v>46053</v>
       </c>
       <c r="R69" s="4">
@@ -5661,11 +5608,10 @@
         <v>66.666666666666671</v>
       </c>
       <c r="T69">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U69">
-        <f t="shared" si="28"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="70" spans="1:21" x14ac:dyDescent="0.25">
@@ -5718,11 +5664,11 @@
         <v>0</v>
       </c>
       <c r="P70" s="2">
-        <f t="shared" si="26"/>
+        <f t="shared" si="22"/>
         <v>1.8871233644010934</v>
       </c>
       <c r="Q70" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="23"/>
         <v>46053</v>
       </c>
       <c r="R70" s="4">
@@ -5734,11 +5680,10 @@
         <v>0</v>
       </c>
       <c r="T70">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U70">
-        <f t="shared" si="28"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="71" spans="1:21" x14ac:dyDescent="0.25">
@@ -5791,11 +5736,11 @@
         <v>0</v>
       </c>
       <c r="P71" s="2">
-        <f t="shared" si="26"/>
+        <f t="shared" si="22"/>
         <v>1.8871233644010934</v>
       </c>
       <c r="Q71" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="23"/>
         <v>46053</v>
       </c>
       <c r="R71" s="4">
@@ -5807,11 +5752,10 @@
         <v>0</v>
       </c>
       <c r="T71">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="U71">
-        <f t="shared" si="28"/>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="72" spans="1:21" x14ac:dyDescent="0.25">
@@ -5864,11 +5808,11 @@
         <v>0</v>
       </c>
       <c r="P72" s="2">
-        <f t="shared" si="26"/>
+        <f t="shared" si="22"/>
         <v>1.8871233644010934</v>
       </c>
       <c r="Q72" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="23"/>
         <v>46053</v>
       </c>
       <c r="R72" s="4">
@@ -5880,11 +5824,10 @@
         <v>0</v>
       </c>
       <c r="T72">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="U72">
-        <f t="shared" si="28"/>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="73" spans="1:21" x14ac:dyDescent="0.25">
@@ -5937,11 +5880,11 @@
         <v>2</v>
       </c>
       <c r="P73" s="2">
-        <f t="shared" si="26"/>
+        <f t="shared" si="22"/>
         <v>1.8871233644010934</v>
       </c>
       <c r="Q73" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="23"/>
         <v>46053</v>
       </c>
       <c r="R73" s="4">
@@ -5953,10 +5896,10 @@
         <v>0</v>
       </c>
       <c r="T73">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U73">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="74" spans="1:21" x14ac:dyDescent="0.25">
@@ -6009,11 +5952,11 @@
         <v>2</v>
       </c>
       <c r="P74" s="2">
-        <f t="shared" si="26"/>
+        <f t="shared" si="22"/>
         <v>1.8871233644010934</v>
       </c>
       <c r="Q74" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="23"/>
         <v>46053</v>
       </c>
       <c r="R74" s="4">
@@ -6025,10 +5968,10 @@
         <v>0</v>
       </c>
       <c r="T74">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U74">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="75" spans="1:21" x14ac:dyDescent="0.25">
@@ -6081,11 +6024,11 @@
         <v>2</v>
       </c>
       <c r="P75" s="2">
-        <f t="shared" si="26"/>
+        <f t="shared" si="22"/>
         <v>1.8871233644010934</v>
       </c>
       <c r="Q75" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="23"/>
         <v>46053</v>
       </c>
       <c r="R75" s="4">
@@ -6097,10 +6040,10 @@
         <v>0</v>
       </c>
       <c r="T75">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U75">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="76" spans="1:21" x14ac:dyDescent="0.25">
@@ -6153,11 +6096,11 @@
         <v>2</v>
       </c>
       <c r="P76" s="2">
-        <f t="shared" si="26"/>
+        <f t="shared" si="22"/>
         <v>1.8871233644010934</v>
       </c>
       <c r="Q76" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="23"/>
         <v>46053</v>
       </c>
       <c r="R76" s="4">
@@ -6169,10 +6112,10 @@
         <v>0</v>
       </c>
       <c r="T76">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U76">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="77" spans="1:21" x14ac:dyDescent="0.25">
@@ -6225,11 +6168,11 @@
         <v>0</v>
       </c>
       <c r="P77" s="2">
-        <f t="shared" si="26"/>
+        <f t="shared" si="22"/>
         <v>1.8871233644010934</v>
       </c>
       <c r="Q77" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="23"/>
         <v>46053</v>
       </c>
       <c r="R77" s="4">
@@ -6241,11 +6184,10 @@
         <v>0</v>
       </c>
       <c r="T77">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U77">
-        <f t="shared" ref="U77:U87" si="29">T77</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="78" spans="1:21" x14ac:dyDescent="0.25">
@@ -6298,11 +6240,11 @@
         <v>0</v>
       </c>
       <c r="P78" s="2">
-        <f t="shared" si="26"/>
+        <f t="shared" si="22"/>
         <v>0.41666666666666669</v>
       </c>
       <c r="Q78" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="23"/>
         <v>46053</v>
       </c>
       <c r="R78" s="4">
@@ -6314,11 +6256,10 @@
         <v>0</v>
       </c>
       <c r="T78">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U78">
-        <f t="shared" si="29"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="79" spans="1:21" x14ac:dyDescent="0.25">
@@ -6371,11 +6312,11 @@
         <v>0</v>
       </c>
       <c r="P79" s="2">
-        <f t="shared" si="26"/>
+        <f t="shared" si="22"/>
         <v>8.5607481788467137</v>
       </c>
       <c r="Q79" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="23"/>
         <v>44592</v>
       </c>
       <c r="R79" s="4">
@@ -6387,11 +6328,10 @@
         <v>0</v>
       </c>
       <c r="T79">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U79">
-        <f t="shared" si="29"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="80" spans="1:21" x14ac:dyDescent="0.25">
@@ -6444,11 +6384,11 @@
         <v>0</v>
       </c>
       <c r="P80" s="2">
-        <f t="shared" si="26"/>
+        <f t="shared" si="22"/>
         <v>5.2216299555219434</v>
       </c>
       <c r="Q80" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="23"/>
         <v>46053</v>
       </c>
       <c r="R80" s="4">
@@ -6460,11 +6400,10 @@
         <v>0</v>
       </c>
       <c r="T80">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U80">
-        <f t="shared" si="29"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="81" spans="1:21" x14ac:dyDescent="0.25">
@@ -6517,11 +6456,11 @@
         <v>0</v>
       </c>
       <c r="P81" s="2">
-        <f t="shared" si="26"/>
+        <f t="shared" si="22"/>
         <v>1.8871233644010934</v>
       </c>
       <c r="Q81" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="23"/>
         <v>46053</v>
       </c>
       <c r="R81" s="4">
@@ -6533,11 +6472,10 @@
         <v>0</v>
       </c>
       <c r="T81">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U81">
-        <f t="shared" si="29"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="82" spans="1:21" x14ac:dyDescent="0.25">
@@ -6589,11 +6527,11 @@
         <v>0</v>
       </c>
       <c r="P82" s="2">
-        <f t="shared" si="26"/>
+        <f t="shared" si="22"/>
         <v>1.8871233644010934</v>
       </c>
       <c r="Q82" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="23"/>
         <v>46053</v>
       </c>
       <c r="R82" s="4">
@@ -6605,11 +6543,10 @@
         <v>142.85714285714286</v>
       </c>
       <c r="T82">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U82">
-        <f t="shared" si="29"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="83" spans="1:21" x14ac:dyDescent="0.25">
@@ -6661,11 +6598,11 @@
         <v>0</v>
       </c>
       <c r="P83" s="2">
-        <f t="shared" si="26"/>
+        <f t="shared" si="22"/>
         <v>1.8871233644010934</v>
       </c>
       <c r="Q83" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="23"/>
         <v>46053</v>
       </c>
       <c r="R83" s="4">
@@ -6677,11 +6614,10 @@
         <v>100</v>
       </c>
       <c r="T83">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U83">
-        <f t="shared" si="29"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="84" spans="1:21" x14ac:dyDescent="0.25">
@@ -6733,11 +6669,11 @@
         <v>0</v>
       </c>
       <c r="P84" s="2">
-        <f t="shared" si="26"/>
+        <f t="shared" si="22"/>
         <v>1.8871233644010934</v>
       </c>
       <c r="Q84" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="23"/>
         <v>46053</v>
       </c>
       <c r="R84" s="4">
@@ -6749,11 +6685,10 @@
         <v>66.666666666666671</v>
       </c>
       <c r="T84">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U84">
-        <f t="shared" si="29"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="85" spans="1:21" x14ac:dyDescent="0.25">
@@ -6806,11 +6741,11 @@
         <v>0</v>
       </c>
       <c r="P85" s="2">
-        <f t="shared" si="26"/>
+        <f t="shared" si="22"/>
         <v>1.8871233644010934</v>
       </c>
       <c r="Q85" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="23"/>
         <v>46053</v>
       </c>
       <c r="R85" s="4">
@@ -6822,11 +6757,10 @@
         <v>0</v>
       </c>
       <c r="T85">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U85">
-        <f t="shared" si="29"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="86" spans="1:21" x14ac:dyDescent="0.25">
@@ -6879,11 +6813,11 @@
         <v>0</v>
       </c>
       <c r="P86" s="2">
-        <f t="shared" si="26"/>
+        <f t="shared" si="22"/>
         <v>1.8871233644010934</v>
       </c>
       <c r="Q86" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="23"/>
         <v>46053</v>
       </c>
       <c r="R86" s="4">
@@ -6895,11 +6829,10 @@
         <v>0</v>
       </c>
       <c r="T86">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="U86">
-        <f t="shared" si="29"/>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="87" spans="1:21" x14ac:dyDescent="0.25">
@@ -6952,11 +6885,11 @@
         <v>0</v>
       </c>
       <c r="P87" s="2">
-        <f t="shared" si="26"/>
+        <f t="shared" si="22"/>
         <v>1.8871233644010934</v>
       </c>
       <c r="Q87" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="23"/>
         <v>46053</v>
       </c>
       <c r="R87" s="4">
@@ -6968,11 +6901,10 @@
         <v>0</v>
       </c>
       <c r="T87">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="U87">
-        <f t="shared" si="29"/>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="88" spans="1:21" x14ac:dyDescent="0.25">
@@ -7025,11 +6957,11 @@
         <v>2</v>
       </c>
       <c r="P88" s="2">
-        <f t="shared" si="26"/>
+        <f t="shared" si="22"/>
         <v>1.8871233644010934</v>
       </c>
       <c r="Q88" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="23"/>
         <v>46053</v>
       </c>
       <c r="R88" s="4">
@@ -7041,10 +6973,10 @@
         <v>0</v>
       </c>
       <c r="T88">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U88">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="89" spans="1:21" x14ac:dyDescent="0.25">
@@ -7097,11 +7029,11 @@
         <v>2</v>
       </c>
       <c r="P89" s="2">
-        <f t="shared" si="26"/>
+        <f t="shared" si="22"/>
         <v>1.8871233644010934</v>
       </c>
       <c r="Q89" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="23"/>
         <v>46053</v>
       </c>
       <c r="R89" s="4">
@@ -7113,10 +7045,10 @@
         <v>0</v>
       </c>
       <c r="T89">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U89">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="90" spans="1:21" x14ac:dyDescent="0.25">
@@ -7169,11 +7101,11 @@
         <v>2</v>
       </c>
       <c r="P90" s="2">
-        <f t="shared" si="26"/>
+        <f t="shared" si="22"/>
         <v>1.8871233644010934</v>
       </c>
       <c r="Q90" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="23"/>
         <v>46053</v>
       </c>
       <c r="R90" s="4">
@@ -7185,10 +7117,10 @@
         <v>0</v>
       </c>
       <c r="T90">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U90">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="91" spans="1:21" x14ac:dyDescent="0.25">
@@ -7241,11 +7173,11 @@
         <v>2</v>
       </c>
       <c r="P91" s="2">
-        <f t="shared" si="26"/>
+        <f t="shared" si="22"/>
         <v>1.8871233644010934</v>
       </c>
       <c r="Q91" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="23"/>
         <v>46053</v>
       </c>
       <c r="R91" s="4">
@@ -7257,10 +7189,10 @@
         <v>0</v>
       </c>
       <c r="T91">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U91">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="92" spans="1:21" x14ac:dyDescent="0.25">
@@ -7313,11 +7245,11 @@
         <v>0</v>
       </c>
       <c r="P92" s="2">
-        <f t="shared" si="26"/>
+        <f t="shared" si="22"/>
         <v>1.8871233644010934</v>
       </c>
       <c r="Q92" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="23"/>
         <v>46053</v>
       </c>
       <c r="R92" s="4">
@@ -7329,11 +7261,10 @@
         <v>0</v>
       </c>
       <c r="T92">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U92">
-        <f t="shared" ref="U92:U102" si="30">T92</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="93" spans="1:21" x14ac:dyDescent="0.25">
@@ -7386,11 +7317,11 @@
         <v>0</v>
       </c>
       <c r="P93" s="2">
-        <f t="shared" si="26"/>
+        <f t="shared" si="22"/>
         <v>0.41666666666666669</v>
       </c>
       <c r="Q93" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="23"/>
         <v>46053</v>
       </c>
       <c r="R93" s="4">
@@ -7402,11 +7333,10 @@
         <v>0</v>
       </c>
       <c r="T93">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U93">
-        <f t="shared" si="30"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="94" spans="1:21" x14ac:dyDescent="0.25">
@@ -7459,11 +7389,11 @@
         <v>0</v>
       </c>
       <c r="P94" s="2">
-        <f t="shared" si="26"/>
+        <f t="shared" si="22"/>
         <v>8.5607481788467137</v>
       </c>
       <c r="Q94" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="23"/>
         <v>44592</v>
       </c>
       <c r="R94" s="4">
@@ -7475,11 +7405,10 @@
         <v>0</v>
       </c>
       <c r="T94">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U94">
-        <f t="shared" si="30"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="95" spans="1:21" x14ac:dyDescent="0.25">
@@ -7532,11 +7461,11 @@
         <v>0</v>
       </c>
       <c r="P95" s="2">
-        <f t="shared" si="26"/>
+        <f t="shared" si="22"/>
         <v>5.2216299555219434</v>
       </c>
       <c r="Q95" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="23"/>
         <v>46053</v>
       </c>
       <c r="R95" s="4">
@@ -7548,11 +7477,10 @@
         <v>0</v>
       </c>
       <c r="T95">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U95">
-        <f t="shared" si="30"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="96" spans="1:21" x14ac:dyDescent="0.25">
@@ -7605,11 +7533,11 @@
         <v>0</v>
       </c>
       <c r="P96" s="2">
-        <f t="shared" si="26"/>
+        <f t="shared" si="22"/>
         <v>1.8871233644010934</v>
       </c>
       <c r="Q96" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="23"/>
         <v>46053</v>
       </c>
       <c r="R96" s="4">
@@ -7621,11 +7549,10 @@
         <v>0</v>
       </c>
       <c r="T96">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U96">
-        <f t="shared" si="30"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="97" spans="1:21" x14ac:dyDescent="0.25">
@@ -7677,11 +7604,11 @@
         <v>0</v>
       </c>
       <c r="P97" s="2">
-        <f t="shared" si="26"/>
+        <f t="shared" si="22"/>
         <v>1.8871233644010934</v>
       </c>
       <c r="Q97" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="23"/>
         <v>46053</v>
       </c>
       <c r="R97" s="4">
@@ -7693,11 +7620,10 @@
         <v>142.85714285714286</v>
       </c>
       <c r="T97">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U97">
-        <f t="shared" si="30"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="98" spans="1:21" x14ac:dyDescent="0.25">
@@ -7749,11 +7675,11 @@
         <v>0</v>
       </c>
       <c r="P98" s="2">
-        <f t="shared" si="26"/>
+        <f t="shared" si="22"/>
         <v>1.8871233644010934</v>
       </c>
       <c r="Q98" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="23"/>
         <v>46053</v>
       </c>
       <c r="R98" s="4">
@@ -7765,11 +7691,10 @@
         <v>100</v>
       </c>
       <c r="T98">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U98">
-        <f t="shared" si="30"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="99" spans="1:21" x14ac:dyDescent="0.25">
@@ -7821,11 +7746,11 @@
         <v>0</v>
       </c>
       <c r="P99" s="2">
-        <f t="shared" si="26"/>
+        <f t="shared" si="22"/>
         <v>1.8871233644010934</v>
       </c>
       <c r="Q99" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="23"/>
         <v>46053</v>
       </c>
       <c r="R99" s="4">
@@ -7837,11 +7762,10 @@
         <v>66.666666666666671</v>
       </c>
       <c r="T99">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U99">
-        <f t="shared" si="30"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="100" spans="1:21" x14ac:dyDescent="0.25">
@@ -7894,11 +7818,11 @@
         <v>0</v>
       </c>
       <c r="P100" s="2">
-        <f t="shared" si="26"/>
+        <f t="shared" si="22"/>
         <v>1.8871233644010934</v>
       </c>
       <c r="Q100" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="23"/>
         <v>46053</v>
       </c>
       <c r="R100" s="4">
@@ -7910,11 +7834,10 @@
         <v>0</v>
       </c>
       <c r="T100">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U100">
-        <f t="shared" si="30"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="101" spans="1:21" x14ac:dyDescent="0.25">
@@ -7967,11 +7890,11 @@
         <v>0</v>
       </c>
       <c r="P101" s="2">
-        <f t="shared" si="26"/>
+        <f t="shared" si="22"/>
         <v>1.8871233644010934</v>
       </c>
       <c r="Q101" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="23"/>
         <v>46053</v>
       </c>
       <c r="R101" s="4">
@@ -7983,11 +7906,10 @@
         <v>0</v>
       </c>
       <c r="T101">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="U101">
-        <f t="shared" si="30"/>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="102" spans="1:21" x14ac:dyDescent="0.25">
@@ -8040,11 +7962,11 @@
         <v>0</v>
       </c>
       <c r="P102" s="2">
-        <f t="shared" si="26"/>
+        <f t="shared" si="22"/>
         <v>1.8871233644010934</v>
       </c>
       <c r="Q102" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="23"/>
         <v>46053</v>
       </c>
       <c r="R102" s="4">
@@ -8056,11 +7978,10 @@
         <v>0</v>
       </c>
       <c r="T102">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="U102">
-        <f t="shared" si="30"/>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="103" spans="1:21" x14ac:dyDescent="0.25">
@@ -8113,11 +8034,11 @@
         <v>2</v>
       </c>
       <c r="P103" s="2">
-        <f t="shared" si="26"/>
+        <f t="shared" si="22"/>
         <v>1.8871233644010934</v>
       </c>
       <c r="Q103" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="23"/>
         <v>46053</v>
       </c>
       <c r="R103" s="4">
@@ -8129,10 +8050,10 @@
         <v>0</v>
       </c>
       <c r="T103">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U103">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="104" spans="1:21" x14ac:dyDescent="0.25">
@@ -8185,11 +8106,11 @@
         <v>2</v>
       </c>
       <c r="P104" s="2">
-        <f t="shared" si="26"/>
+        <f t="shared" si="22"/>
         <v>1.8871233644010934</v>
       </c>
       <c r="Q104" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="23"/>
         <v>46053</v>
       </c>
       <c r="R104" s="4">
@@ -8201,10 +8122,10 @@
         <v>0</v>
       </c>
       <c r="T104">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U104">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="105" spans="1:21" x14ac:dyDescent="0.25">
@@ -8257,11 +8178,11 @@
         <v>2</v>
       </c>
       <c r="P105" s="2">
-        <f t="shared" si="26"/>
+        <f t="shared" si="22"/>
         <v>1.8871233644010934</v>
       </c>
       <c r="Q105" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="23"/>
         <v>46053</v>
       </c>
       <c r="R105" s="4">
@@ -8273,10 +8194,10 @@
         <v>0</v>
       </c>
       <c r="T105">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U105">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="106" spans="1:21" x14ac:dyDescent="0.25">
@@ -8329,11 +8250,11 @@
         <v>2</v>
       </c>
       <c r="P106" s="2">
-        <f t="shared" si="26"/>
+        <f t="shared" si="22"/>
         <v>1.8871233644010934</v>
       </c>
       <c r="Q106" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="23"/>
         <v>46053</v>
       </c>
       <c r="R106" s="4">
@@ -8345,10 +8266,10 @@
         <v>0</v>
       </c>
       <c r="T106">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U106">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="107" spans="1:21" x14ac:dyDescent="0.25">
@@ -8401,11 +8322,11 @@
         <v>0</v>
       </c>
       <c r="P107" s="2">
-        <f t="shared" si="26"/>
+        <f t="shared" si="22"/>
         <v>1.8871233644010934</v>
       </c>
       <c r="Q107" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="23"/>
         <v>46053</v>
       </c>
       <c r="R107" s="4">
@@ -8417,11 +8338,10 @@
         <v>0</v>
       </c>
       <c r="T107">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U107">
-        <f t="shared" ref="U107:U117" si="31">T107</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="108" spans="1:21" x14ac:dyDescent="0.25">
@@ -8474,11 +8394,11 @@
         <v>0</v>
       </c>
       <c r="P108" s="2">
-        <f t="shared" si="26"/>
+        <f t="shared" si="22"/>
         <v>0.41666666666666669</v>
       </c>
       <c r="Q108" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="23"/>
         <v>46053</v>
       </c>
       <c r="R108" s="4">
@@ -8490,11 +8410,10 @@
         <v>0</v>
       </c>
       <c r="T108">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U108">
-        <f t="shared" si="31"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="109" spans="1:21" x14ac:dyDescent="0.25">
@@ -8547,11 +8466,11 @@
         <v>0</v>
       </c>
       <c r="P109" s="2">
-        <f t="shared" si="26"/>
+        <f t="shared" si="22"/>
         <v>8.5607481788467137</v>
       </c>
       <c r="Q109" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="23"/>
         <v>44592</v>
       </c>
       <c r="R109" s="4">
@@ -8563,11 +8482,10 @@
         <v>0</v>
       </c>
       <c r="T109">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U109">
-        <f t="shared" si="31"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="110" spans="1:21" x14ac:dyDescent="0.25">
@@ -8620,11 +8538,11 @@
         <v>0</v>
       </c>
       <c r="P110" s="2">
-        <f t="shared" si="26"/>
+        <f t="shared" si="22"/>
         <v>5.2216299555219434</v>
       </c>
       <c r="Q110" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="23"/>
         <v>46053</v>
       </c>
       <c r="R110" s="4">
@@ -8636,11 +8554,10 @@
         <v>0</v>
       </c>
       <c r="T110">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U110">
-        <f t="shared" si="31"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="111" spans="1:21" x14ac:dyDescent="0.25">
@@ -8693,11 +8610,11 @@
         <v>0</v>
       </c>
       <c r="P111" s="2">
-        <f t="shared" si="26"/>
+        <f t="shared" si="22"/>
         <v>1.8871233644010934</v>
       </c>
       <c r="Q111" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="23"/>
         <v>46053</v>
       </c>
       <c r="R111" s="4">
@@ -8709,11 +8626,10 @@
         <v>0</v>
       </c>
       <c r="T111">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U111">
-        <f t="shared" si="31"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="112" spans="1:21" x14ac:dyDescent="0.25">
@@ -8765,11 +8681,11 @@
         <v>0</v>
       </c>
       <c r="P112" s="2">
-        <f t="shared" si="26"/>
+        <f t="shared" si="22"/>
         <v>1.8871233644010934</v>
       </c>
       <c r="Q112" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="23"/>
         <v>46053</v>
       </c>
       <c r="R112" s="4">
@@ -8781,11 +8697,10 @@
         <v>142.85714285714286</v>
       </c>
       <c r="T112">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U112">
-        <f t="shared" si="31"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="113" spans="1:21" x14ac:dyDescent="0.25">
@@ -8837,11 +8752,11 @@
         <v>0</v>
       </c>
       <c r="P113" s="2">
-        <f t="shared" si="26"/>
+        <f t="shared" si="22"/>
         <v>1.8871233644010934</v>
       </c>
       <c r="Q113" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="23"/>
         <v>46053</v>
       </c>
       <c r="R113" s="4">
@@ -8853,11 +8768,10 @@
         <v>100</v>
       </c>
       <c r="T113">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U113">
-        <f t="shared" si="31"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="114" spans="1:21" x14ac:dyDescent="0.25">
@@ -8909,11 +8823,11 @@
         <v>0</v>
       </c>
       <c r="P114" s="2">
-        <f t="shared" si="26"/>
+        <f t="shared" si="22"/>
         <v>1.8871233644010934</v>
       </c>
       <c r="Q114" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="23"/>
         <v>46053</v>
       </c>
       <c r="R114" s="4">
@@ -8925,11 +8839,10 @@
         <v>66.666666666666671</v>
       </c>
       <c r="T114">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U114">
-        <f t="shared" si="31"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="115" spans="1:21" x14ac:dyDescent="0.25">
@@ -8982,11 +8895,11 @@
         <v>0</v>
       </c>
       <c r="P115" s="2">
-        <f t="shared" si="26"/>
+        <f t="shared" si="22"/>
         <v>1.8871233644010934</v>
       </c>
       <c r="Q115" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="23"/>
         <v>46053</v>
       </c>
       <c r="R115" s="4">
@@ -8998,11 +8911,10 @@
         <v>0</v>
       </c>
       <c r="T115">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U115">
-        <f t="shared" si="31"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="116" spans="1:21" x14ac:dyDescent="0.25">
@@ -9055,11 +8967,11 @@
         <v>0</v>
       </c>
       <c r="P116" s="2">
-        <f t="shared" si="26"/>
+        <f t="shared" si="22"/>
         <v>1.8871233644010934</v>
       </c>
       <c r="Q116" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="23"/>
         <v>46053</v>
       </c>
       <c r="R116" s="4">
@@ -9071,11 +8983,10 @@
         <v>0</v>
       </c>
       <c r="T116">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="U116">
-        <f t="shared" si="31"/>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="117" spans="1:21" x14ac:dyDescent="0.25">
@@ -9128,11 +9039,11 @@
         <v>0</v>
       </c>
       <c r="P117" s="2">
-        <f t="shared" si="26"/>
+        <f t="shared" si="22"/>
         <v>1.8871233644010934</v>
       </c>
       <c r="Q117" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="23"/>
         <v>46053</v>
       </c>
       <c r="R117" s="4">
@@ -9144,11 +9055,10 @@
         <v>0</v>
       </c>
       <c r="T117">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="U117">
-        <f t="shared" si="31"/>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="118" spans="1:21" x14ac:dyDescent="0.25">
@@ -9201,11 +9111,11 @@
         <v>2</v>
       </c>
       <c r="P118" s="2">
-        <f t="shared" si="26"/>
+        <f t="shared" si="22"/>
         <v>1.8871233644010934</v>
       </c>
       <c r="Q118" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="23"/>
         <v>46053</v>
       </c>
       <c r="R118" s="4">
@@ -9217,10 +9127,10 @@
         <v>0</v>
       </c>
       <c r="T118">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U118">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="119" spans="1:21" x14ac:dyDescent="0.25">
@@ -9273,11 +9183,11 @@
         <v>2</v>
       </c>
       <c r="P119" s="2">
-        <f t="shared" si="26"/>
+        <f t="shared" si="22"/>
         <v>1.8871233644010934</v>
       </c>
       <c r="Q119" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="23"/>
         <v>46053</v>
       </c>
       <c r="R119" s="4">
@@ -9289,10 +9199,10 @@
         <v>0</v>
       </c>
       <c r="T119">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U119">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="120" spans="1:21" x14ac:dyDescent="0.25">
@@ -9345,11 +9255,11 @@
         <v>2</v>
       </c>
       <c r="P120" s="2">
-        <f t="shared" si="26"/>
+        <f t="shared" si="22"/>
         <v>1.8871233644010934</v>
       </c>
       <c r="Q120" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="23"/>
         <v>46053</v>
       </c>
       <c r="R120" s="4">
@@ -9361,10 +9271,10 @@
         <v>0</v>
       </c>
       <c r="T120">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U120">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="121" spans="1:21" x14ac:dyDescent="0.25">
@@ -9417,11 +9327,11 @@
         <v>2</v>
       </c>
       <c r="P121" s="2">
-        <f t="shared" ref="P121" si="32">-PMT(M121/K121,DATEDIF(D121,Q121,"y")*I121,E121,-G121,0)</f>
+        <f t="shared" ref="P121" si="24">-PMT(M121/K121,DATEDIF(D121,Q121,"y")*I121,E121,-G121,0)</f>
         <v>1.8871233644010934</v>
       </c>
       <c r="Q121" s="1">
-        <f t="shared" ref="Q121" si="33">EOMONTH(D121,H121)</f>
+        <f t="shared" ref="Q121" si="25">EOMONTH(D121,H121)</f>
         <v>46053</v>
       </c>
       <c r="R121" s="4">
@@ -9433,10 +9343,10 @@
         <v>0</v>
       </c>
       <c r="T121">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U121">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>